<commit_message>
- updated table and picture of PT calcualtions
</commit_message>
<xml_diff>
--- a/doc/pt1000_pt100_pt500_tables.xlsx
+++ b/doc/pt1000_pt100_pt500_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_SELTRON\zigamiklosic\Personal\HomeWork\RND_Thermal_Modeling\src\drivers\devices\thermistor\thermistor\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B0274E-A367-473B-9068-2A7CF8AD41B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718E9F6D-8C8D-4B82-BCA4-99EA934D4FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,9 +185,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -220,6 +217,9 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2920,7 +2920,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="860"/>
-          <c:min val="-210"/>
+          <c:min val="-200"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4124,2044 +4124,2044 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AD238"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A75" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M114" sqref="M114"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y53" sqref="Y53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
     </row>
     <row r="2" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
     </row>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="E3" s="13"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>-200</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>185.2</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <f>C5/10</f>
         <v>18.52</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="14"/>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>-190</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>228.25</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <f t="shared" ref="D6:D69" si="0">C6/10</f>
         <v>22.824999999999999</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>114.13</v>
       </c>
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>-180</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>270.95999999999998</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <f t="shared" si="0"/>
         <v>27.095999999999997</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>135.47999999999999</v>
       </c>
     </row>
     <row r="8" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>-170</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>313.35000000000002</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <f t="shared" si="0"/>
         <v>31.335000000000001</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>156.68</v>
       </c>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>-160</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>355.45</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <f t="shared" si="0"/>
         <v>35.545000000000002</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>177.72</v>
       </c>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>-150</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>397.23</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <f t="shared" si="0"/>
         <v>39.722999999999999</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>198.62</v>
       </c>
     </row>
     <row r="11" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>-140</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>438.76</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <f t="shared" si="0"/>
         <v>43.875999999999998</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>219.38</v>
       </c>
-      <c r="AD11" s="16"/>
+      <c r="AD11" s="15"/>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>-130</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>480.05</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <f t="shared" si="0"/>
         <v>48.005000000000003</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>240.02</v>
       </c>
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>-120</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>521.1</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <f t="shared" si="0"/>
         <v>52.11</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>260.55</v>
       </c>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>-110</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>561.92999999999995</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <f t="shared" si="0"/>
         <v>56.192999999999998</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>280.97000000000003</v>
       </c>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>-100</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>602.55999999999995</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <f t="shared" si="0"/>
         <v>60.255999999999993</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>301.27999999999997</v>
       </c>
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>-90</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>643</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="8">
         <f t="shared" si="0"/>
         <v>64.3</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <v>321.5</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>-80</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>683.25</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <f t="shared" si="0"/>
         <v>68.325000000000003</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>341.63</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>-70</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>723.35</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <f t="shared" si="0"/>
         <v>72.335000000000008</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="9">
         <v>361.67</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>-60</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <v>763.28</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <f t="shared" si="0"/>
         <v>76.328000000000003</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="9">
         <v>381.64</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>-50</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>803.06</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <f t="shared" si="0"/>
         <v>80.305999999999997</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="9">
         <v>401.53</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>-40</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>842.71</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="8">
         <f t="shared" si="0"/>
         <v>84.271000000000001</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="9">
         <v>421.35</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>-30</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>882.22</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="8">
         <f t="shared" si="0"/>
         <v>88.222000000000008</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="9">
         <v>441.11</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <v>-20</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="9">
         <v>921.6</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="8">
         <f t="shared" si="0"/>
         <v>92.16</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="9">
         <v>460.8</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <v>-10</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="9">
         <v>960.86</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="8">
         <f t="shared" si="0"/>
         <v>96.085999999999999</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="9">
         <v>480.43</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <v>0</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="9">
         <v>1000</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="8">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="9">
         <v>500</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <v>10</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="9">
         <v>1039.03</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="8">
         <f t="shared" si="0"/>
         <v>103.90299999999999</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="9">
         <v>519.51</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <v>20</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="9">
         <v>1077.94</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="8">
         <f t="shared" si="0"/>
         <v>107.79400000000001</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="9">
         <v>538.97</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="7">
+      <c r="B28" s="6">
         <v>30</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="9">
         <v>1116.73</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="8">
         <f t="shared" si="0"/>
         <v>111.673</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="9">
         <v>558.36</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="7">
+      <c r="B29" s="6">
         <v>40</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="9">
         <v>1155.4100000000001</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="8">
         <f t="shared" si="0"/>
         <v>115.54100000000001</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="9">
         <v>577.70000000000005</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="7">
+      <c r="B30" s="6">
         <v>50</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="9">
         <v>1193.97</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="8">
         <f t="shared" si="0"/>
         <v>119.39700000000001</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="9">
         <v>596.99</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="7">
+      <c r="B31" s="6">
         <v>60</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="9">
         <v>1232.42</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="8">
         <f t="shared" si="0"/>
         <v>123.242</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="9">
         <v>616.21</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="7">
+      <c r="B32" s="6">
         <v>70</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="9">
         <v>1270.75</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="8">
         <f t="shared" si="0"/>
         <v>127.075</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="9">
         <v>635.38</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="7">
+      <c r="B33" s="6">
         <v>80</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="9">
         <v>1308.97</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="8">
         <f t="shared" si="0"/>
         <v>130.89699999999999</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="9">
         <v>654.48</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="7">
+      <c r="B34" s="6">
         <v>90</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="9">
         <v>1347.07</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D34" s="8">
         <f t="shared" si="0"/>
         <v>134.70699999999999</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="9">
         <v>673.53</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="7">
+      <c r="B35" s="6">
         <v>100</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="9">
         <v>1385.06</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="8">
         <f t="shared" si="0"/>
         <v>138.506</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="9">
         <v>692.53</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="7">
+      <c r="B36" s="6">
         <v>110</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="9">
         <v>1422.93</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="8">
         <f t="shared" si="0"/>
         <v>142.29300000000001</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="9">
         <v>711.46</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="7">
+      <c r="B37" s="6">
         <v>120</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="9">
         <v>1460.68</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="8">
         <f t="shared" si="0"/>
         <v>146.06800000000001</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37" s="9">
         <v>730.34</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="7">
+      <c r="B38" s="6">
         <v>130</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="9">
         <v>1498.32</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="8">
         <f t="shared" si="0"/>
         <v>149.83199999999999</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E38" s="9">
         <v>749.16</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="7">
+      <c r="B39" s="6">
         <v>140</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="9">
         <v>1535.84</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="8">
         <f t="shared" si="0"/>
         <v>153.584</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E39" s="9">
         <v>767.92</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="7">
+      <c r="B40" s="6">
         <v>150</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="9">
         <v>1573.25</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40" s="8">
         <f t="shared" si="0"/>
         <v>157.32499999999999</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E40" s="9">
         <v>786.63</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="7">
+      <c r="B41" s="6">
         <v>160</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="9">
         <v>1610.54</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="8">
         <f t="shared" si="0"/>
         <v>161.054</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E41" s="9">
         <v>805.27</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="7">
+      <c r="B42" s="6">
         <v>170</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="9">
         <v>1647.72</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42" s="8">
         <f t="shared" si="0"/>
         <v>164.77199999999999</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42" s="9">
         <v>823.86</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="7">
+      <c r="B43" s="6">
         <v>180</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="9">
         <v>1684.78</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D43" s="8">
         <f t="shared" si="0"/>
         <v>168.47800000000001</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43" s="9">
         <v>842.39</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="7">
+      <c r="B44" s="6">
         <v>190</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="9">
         <v>1721.73</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44" s="8">
         <f t="shared" si="0"/>
         <v>172.173</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="9">
         <v>860.86</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="7">
+      <c r="B45" s="6">
         <v>200</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="9">
         <v>1758.56</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D45" s="8">
         <f t="shared" si="0"/>
         <v>175.85599999999999</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="9">
         <v>879.28</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="7">
+      <c r="B46" s="6">
         <v>210</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="9">
         <v>1795.28</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46" s="8">
         <f t="shared" si="0"/>
         <v>179.52799999999999</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E46" s="9">
         <v>897.64</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="7">
+      <c r="B47" s="6">
         <v>220</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="9">
         <v>1831.88</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D47" s="8">
         <f t="shared" si="0"/>
         <v>183.18800000000002</v>
       </c>
-      <c r="E47" s="10">
+      <c r="E47" s="9">
         <v>915.94</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="7">
+      <c r="B48" s="6">
         <v>230</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C48" s="9">
         <v>1868.36</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D48" s="8">
         <f t="shared" si="0"/>
         <v>186.83599999999998</v>
       </c>
-      <c r="E48" s="10">
+      <c r="E48" s="9">
         <v>934.18</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="7">
+      <c r="B49" s="6">
         <v>240</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C49" s="9">
         <v>1904.73</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D49" s="8">
         <f t="shared" si="0"/>
         <v>190.47300000000001</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E49" s="9">
         <v>952.36</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="7">
+      <c r="B50" s="6">
         <v>250</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C50" s="9">
         <v>1940.98</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50" s="8">
         <f t="shared" si="0"/>
         <v>194.09800000000001</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E50" s="9">
         <v>970.49</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="7">
+      <c r="B51" s="6">
         <v>260</v>
       </c>
-      <c r="C51" s="10">
+      <c r="C51" s="9">
         <v>1977.12</v>
       </c>
-      <c r="D51" s="9">
+      <c r="D51" s="8">
         <f t="shared" si="0"/>
         <v>197.71199999999999</v>
       </c>
-      <c r="E51" s="10">
+      <c r="E51" s="9">
         <v>988.56</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="7">
+      <c r="B52" s="6">
         <v>270</v>
       </c>
-      <c r="C52" s="10">
+      <c r="C52" s="9">
         <v>2013.14</v>
       </c>
-      <c r="D52" s="9">
+      <c r="D52" s="8">
         <f t="shared" si="0"/>
         <v>201.31400000000002</v>
       </c>
-      <c r="E52" s="10">
+      <c r="E52" s="9">
         <v>1006.57</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="7">
+      <c r="B53" s="6">
         <v>280</v>
       </c>
-      <c r="C53" s="10">
+      <c r="C53" s="9">
         <v>2049.0500000000002</v>
       </c>
-      <c r="D53" s="9">
+      <c r="D53" s="8">
         <f t="shared" si="0"/>
         <v>204.90500000000003</v>
       </c>
-      <c r="E53" s="10">
+      <c r="E53" s="9">
         <v>1024.52</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="7">
+      <c r="B54" s="6">
         <v>290</v>
       </c>
-      <c r="C54" s="10">
+      <c r="C54" s="9">
         <v>2084.84</v>
       </c>
-      <c r="D54" s="9">
+      <c r="D54" s="8">
         <f t="shared" si="0"/>
         <v>208.48400000000001</v>
       </c>
-      <c r="E54" s="10">
+      <c r="E54" s="9">
         <v>1042.42</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="7">
+      <c r="B55" s="6">
         <v>300</v>
       </c>
-      <c r="C55" s="10">
+      <c r="C55" s="9">
         <v>2120.52</v>
       </c>
-      <c r="D55" s="9">
+      <c r="D55" s="8">
         <f t="shared" si="0"/>
         <v>212.05199999999999</v>
       </c>
-      <c r="E55" s="10">
+      <c r="E55" s="9">
         <v>1060.26</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="7">
+      <c r="B56" s="6">
         <v>310</v>
       </c>
-      <c r="C56" s="10">
+      <c r="C56" s="9">
         <v>2156.08</v>
       </c>
-      <c r="D56" s="9">
+      <c r="D56" s="8">
         <f t="shared" si="0"/>
         <v>215.608</v>
       </c>
-      <c r="E56" s="10">
+      <c r="E56" s="9">
         <v>1078.04</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="7">
+      <c r="B57" s="6">
         <v>320</v>
       </c>
-      <c r="C57" s="10">
+      <c r="C57" s="9">
         <v>2191.52</v>
       </c>
-      <c r="D57" s="9">
+      <c r="D57" s="8">
         <f t="shared" si="0"/>
         <v>219.15199999999999</v>
       </c>
-      <c r="E57" s="10">
+      <c r="E57" s="9">
         <v>1095.76</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="7">
+      <c r="B58" s="6">
         <v>330</v>
       </c>
-      <c r="C58" s="10">
+      <c r="C58" s="9">
         <v>2226.85</v>
       </c>
-      <c r="D58" s="9">
+      <c r="D58" s="8">
         <f t="shared" si="0"/>
         <v>222.685</v>
       </c>
-      <c r="E58" s="10">
+      <c r="E58" s="9">
         <v>1113.42</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="7">
+      <c r="B59" s="6">
         <v>340</v>
       </c>
-      <c r="C59" s="10">
+      <c r="C59" s="9">
         <v>2262.06</v>
       </c>
-      <c r="D59" s="9">
+      <c r="D59" s="8">
         <f t="shared" si="0"/>
         <v>226.20599999999999</v>
       </c>
-      <c r="E59" s="10">
+      <c r="E59" s="9">
         <v>1131.03</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="7">
+      <c r="B60" s="6">
         <v>350</v>
       </c>
-      <c r="C60" s="10">
+      <c r="C60" s="9">
         <v>2297.16</v>
       </c>
-      <c r="D60" s="9">
+      <c r="D60" s="8">
         <f t="shared" si="0"/>
         <v>229.71599999999998</v>
       </c>
-      <c r="E60" s="10">
+      <c r="E60" s="9">
         <v>1148.58</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="7">
+      <c r="B61" s="6">
         <v>360</v>
       </c>
-      <c r="C61" s="10">
+      <c r="C61" s="9">
         <v>2332.14</v>
       </c>
-      <c r="D61" s="9">
+      <c r="D61" s="8">
         <f t="shared" si="0"/>
         <v>233.214</v>
       </c>
-      <c r="E61" s="10">
+      <c r="E61" s="9">
         <v>1166.07</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="7">
+      <c r="B62" s="6">
         <v>370</v>
       </c>
-      <c r="C62" s="10">
+      <c r="C62" s="9">
         <v>2367.0100000000002</v>
       </c>
-      <c r="D62" s="9">
+      <c r="D62" s="8">
         <f t="shared" si="0"/>
         <v>236.70100000000002</v>
       </c>
-      <c r="E62" s="10">
+      <c r="E62" s="9">
         <v>1183.51</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="7">
+      <c r="B63" s="6">
         <v>380</v>
       </c>
-      <c r="C63" s="10">
+      <c r="C63" s="9">
         <v>2401.7600000000002</v>
       </c>
-      <c r="D63" s="9">
+      <c r="D63" s="8">
         <f t="shared" si="0"/>
         <v>240.17600000000002</v>
       </c>
-      <c r="E63" s="10">
+      <c r="E63" s="9">
         <v>1200.8800000000001</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="7">
+      <c r="B64" s="6">
         <v>390</v>
       </c>
-      <c r="C64" s="10">
+      <c r="C64" s="9">
         <v>2436.4</v>
       </c>
-      <c r="D64" s="9">
+      <c r="D64" s="8">
         <f t="shared" si="0"/>
         <v>243.64000000000001</v>
       </c>
-      <c r="E64" s="10">
+      <c r="E64" s="9">
         <v>1218.2</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="7">
+      <c r="B65" s="6">
         <v>400</v>
       </c>
-      <c r="C65" s="10">
+      <c r="C65" s="9">
         <v>2470.92</v>
       </c>
-      <c r="D65" s="9">
+      <c r="D65" s="8">
         <f t="shared" si="0"/>
         <v>247.09200000000001</v>
       </c>
-      <c r="E65" s="10">
+      <c r="E65" s="9">
         <v>1235.46</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="7">
+      <c r="B66" s="6">
         <v>410</v>
       </c>
-      <c r="C66" s="10">
+      <c r="C66" s="9">
         <v>2505.33</v>
       </c>
-      <c r="D66" s="9">
+      <c r="D66" s="8">
         <f t="shared" si="0"/>
         <v>250.53299999999999</v>
       </c>
-      <c r="E66" s="10">
+      <c r="E66" s="9">
         <v>1252.6600000000001</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="7">
+      <c r="B67" s="6">
         <v>420</v>
       </c>
-      <c r="C67" s="10">
+      <c r="C67" s="9">
         <v>2539.62</v>
       </c>
-      <c r="D67" s="9">
+      <c r="D67" s="8">
         <f t="shared" si="0"/>
         <v>253.96199999999999</v>
       </c>
-      <c r="E67" s="10">
+      <c r="E67" s="9">
         <v>1269.81</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="7">
+      <c r="B68" s="6">
         <v>430</v>
       </c>
-      <c r="C68" s="10">
+      <c r="C68" s="9">
         <v>2573.79</v>
       </c>
-      <c r="D68" s="9">
+      <c r="D68" s="8">
         <f t="shared" si="0"/>
         <v>257.37900000000002</v>
       </c>
-      <c r="E68" s="10">
+      <c r="E68" s="9">
         <v>1286.8900000000001</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="7">
+      <c r="B69" s="6">
         <v>440</v>
       </c>
-      <c r="C69" s="10">
+      <c r="C69" s="9">
         <v>2607.85</v>
       </c>
-      <c r="D69" s="9">
+      <c r="D69" s="8">
         <f t="shared" si="0"/>
         <v>260.78499999999997</v>
       </c>
-      <c r="E69" s="10">
+      <c r="E69" s="9">
         <v>1303.92</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="7">
+      <c r="B70" s="6">
         <v>450</v>
       </c>
-      <c r="C70" s="10">
+      <c r="C70" s="9">
         <v>2641.79</v>
       </c>
-      <c r="D70" s="9">
+      <c r="D70" s="8">
         <f t="shared" ref="D70:D110" si="1">C70/10</f>
         <v>264.17899999999997</v>
       </c>
-      <c r="E70" s="10">
+      <c r="E70" s="9">
         <v>1320.9</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="7">
+      <c r="B71" s="6">
         <v>460</v>
       </c>
-      <c r="C71" s="10">
+      <c r="C71" s="9">
         <v>2675.62</v>
       </c>
-      <c r="D71" s="9">
+      <c r="D71" s="8">
         <f t="shared" si="1"/>
         <v>267.56200000000001</v>
       </c>
-      <c r="E71" s="10">
+      <c r="E71" s="9">
         <v>1337.81</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="7">
+      <c r="B72" s="6">
         <v>470</v>
       </c>
-      <c r="C72" s="10">
+      <c r="C72" s="9">
         <v>2709.33</v>
       </c>
-      <c r="D72" s="9">
+      <c r="D72" s="8">
         <f t="shared" si="1"/>
         <v>270.93299999999999</v>
       </c>
-      <c r="E72" s="10">
+      <c r="E72" s="9">
         <v>1354.67</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="7">
+      <c r="B73" s="6">
         <v>480</v>
       </c>
-      <c r="C73" s="10">
+      <c r="C73" s="9">
         <v>2742.93</v>
       </c>
-      <c r="D73" s="9">
+      <c r="D73" s="8">
         <f t="shared" si="1"/>
         <v>274.29300000000001</v>
       </c>
-      <c r="E73" s="10">
+      <c r="E73" s="9">
         <v>1371.46</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="7">
+      <c r="B74" s="6">
         <v>490</v>
       </c>
-      <c r="C74" s="10">
+      <c r="C74" s="9">
         <v>2776.41</v>
       </c>
-      <c r="D74" s="9">
+      <c r="D74" s="8">
         <f t="shared" si="1"/>
         <v>277.64099999999996</v>
       </c>
-      <c r="E74" s="10">
+      <c r="E74" s="9">
         <v>1388.2</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="7">
+      <c r="B75" s="6">
         <v>500</v>
       </c>
-      <c r="C75" s="10">
+      <c r="C75" s="9">
         <v>2809.78</v>
       </c>
-      <c r="D75" s="9">
+      <c r="D75" s="8">
         <f t="shared" si="1"/>
         <v>280.97800000000001</v>
       </c>
-      <c r="E75" s="10">
+      <c r="E75" s="9">
         <v>1404.89</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="7">
+      <c r="B76" s="6">
         <v>510</v>
       </c>
-      <c r="C76" s="10">
+      <c r="C76" s="9">
         <v>2843.03</v>
       </c>
-      <c r="D76" s="9">
+      <c r="D76" s="8">
         <f t="shared" si="1"/>
         <v>284.303</v>
       </c>
-      <c r="E76" s="10">
+      <c r="E76" s="9">
         <v>1421.51</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="7">
+      <c r="B77" s="6">
         <v>520</v>
       </c>
-      <c r="C77" s="10">
+      <c r="C77" s="9">
         <v>2876.16</v>
       </c>
-      <c r="D77" s="9">
+      <c r="D77" s="8">
         <f t="shared" si="1"/>
         <v>287.61599999999999</v>
       </c>
-      <c r="E77" s="10">
+      <c r="E77" s="9">
         <v>1438.08</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="7">
+      <c r="B78" s="6">
         <v>530</v>
       </c>
-      <c r="C78" s="10">
+      <c r="C78" s="9">
         <v>2909.18</v>
       </c>
-      <c r="D78" s="9">
+      <c r="D78" s="8">
         <f t="shared" si="1"/>
         <v>290.91800000000001</v>
       </c>
-      <c r="E78" s="10">
+      <c r="E78" s="9">
         <v>1454.59</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="7">
+      <c r="B79" s="6">
         <v>540</v>
       </c>
-      <c r="C79" s="10">
+      <c r="C79" s="9">
         <v>2942.08</v>
       </c>
-      <c r="D79" s="9">
+      <c r="D79" s="8">
         <f t="shared" si="1"/>
         <v>294.20799999999997</v>
       </c>
-      <c r="E79" s="10">
+      <c r="E79" s="9">
         <v>1471.04</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="7">
+      <c r="B80" s="6">
         <v>550</v>
       </c>
-      <c r="C80" s="10">
+      <c r="C80" s="9">
         <v>2974.87</v>
       </c>
-      <c r="D80" s="9">
+      <c r="D80" s="8">
         <f t="shared" si="1"/>
         <v>297.48699999999997</v>
       </c>
-      <c r="E80" s="10">
+      <c r="E80" s="9">
         <v>1487.44</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="7">
+      <c r="B81" s="6">
         <v>560</v>
       </c>
-      <c r="C81" s="10">
+      <c r="C81" s="9">
         <v>3007.54</v>
       </c>
-      <c r="D81" s="9">
+      <c r="D81" s="8">
         <f t="shared" si="1"/>
         <v>300.75400000000002</v>
       </c>
-      <c r="E81" s="10">
+      <c r="E81" s="9">
         <v>1503.77</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="7">
+      <c r="B82" s="6">
         <v>570</v>
       </c>
-      <c r="C82" s="10">
+      <c r="C82" s="9">
         <v>3040.1</v>
       </c>
-      <c r="D82" s="9">
+      <c r="D82" s="8">
         <f t="shared" si="1"/>
         <v>304.01</v>
       </c>
-      <c r="E82" s="10">
+      <c r="E82" s="9">
         <v>1520.05</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="7">
+      <c r="B83" s="6">
         <v>580</v>
       </c>
-      <c r="C83" s="10">
+      <c r="C83" s="9">
         <v>3078.54</v>
       </c>
-      <c r="D83" s="9">
+      <c r="D83" s="8">
         <f t="shared" si="1"/>
         <v>307.85399999999998</v>
       </c>
-      <c r="E83" s="10">
+      <c r="E83" s="9">
         <v>1536.27</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="7">
+      <c r="B84" s="6">
         <v>590</v>
       </c>
-      <c r="C84" s="10">
+      <c r="C84" s="9">
         <v>3104.87</v>
       </c>
-      <c r="D84" s="9">
+      <c r="D84" s="8">
         <f t="shared" si="1"/>
         <v>310.48699999999997</v>
       </c>
-      <c r="E84" s="10">
+      <c r="E84" s="9">
         <v>1552.43</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="7">
+      <c r="B85" s="6">
         <v>600</v>
       </c>
-      <c r="C85" s="10">
+      <c r="C85" s="9">
         <v>3137.08</v>
       </c>
-      <c r="D85" s="9">
+      <c r="D85" s="8">
         <f t="shared" si="1"/>
         <v>313.70799999999997</v>
       </c>
-      <c r="E85" s="10">
+      <c r="E85" s="9">
         <v>1568.54</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="7">
+      <c r="B86" s="6">
         <v>610</v>
       </c>
-      <c r="C86" s="10">
+      <c r="C86" s="9">
         <v>3169.18</v>
       </c>
-      <c r="D86" s="9">
+      <c r="D86" s="8">
         <f t="shared" si="1"/>
         <v>316.91800000000001</v>
       </c>
-      <c r="E86" s="10">
+      <c r="E86" s="9">
         <v>1584.59</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="7">
+      <c r="B87" s="6">
         <v>620</v>
       </c>
-      <c r="C87" s="10">
+      <c r="C87" s="9">
         <v>3201.16</v>
       </c>
-      <c r="D87" s="9">
+      <c r="D87" s="8">
         <f t="shared" si="1"/>
         <v>320.11599999999999</v>
       </c>
-      <c r="E87" s="10">
+      <c r="E87" s="9">
         <v>1600.58</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="7">
+      <c r="B88" s="6">
         <v>630</v>
       </c>
-      <c r="C88" s="10">
+      <c r="C88" s="9">
         <v>3233.02</v>
       </c>
-      <c r="D88" s="9">
+      <c r="D88" s="8">
         <f t="shared" si="1"/>
         <v>323.30200000000002</v>
       </c>
-      <c r="E88" s="10">
+      <c r="E88" s="9">
         <v>1616.51</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B89" s="7">
+      <c r="B89" s="6">
         <v>640</v>
       </c>
-      <c r="C89" s="10">
+      <c r="C89" s="9">
         <v>3264.77</v>
       </c>
-      <c r="D89" s="9">
+      <c r="D89" s="8">
         <f t="shared" si="1"/>
         <v>326.47699999999998</v>
       </c>
-      <c r="E89" s="10">
+      <c r="E89" s="9">
         <v>1632.38</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="7">
+      <c r="B90" s="6">
         <v>650</v>
       </c>
-      <c r="C90" s="10">
+      <c r="C90" s="9">
         <v>3296.4</v>
       </c>
-      <c r="D90" s="9">
+      <c r="D90" s="8">
         <f t="shared" si="1"/>
         <v>329.64</v>
       </c>
-      <c r="E90" s="10">
+      <c r="E90" s="9">
         <v>1648.2</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B91" s="7">
+      <c r="B91" s="6">
         <v>660</v>
       </c>
-      <c r="C91" s="10">
+      <c r="C91" s="9">
         <v>3327.92</v>
       </c>
-      <c r="D91" s="9">
+      <c r="D91" s="8">
         <f t="shared" si="1"/>
         <v>332.79200000000003</v>
       </c>
-      <c r="E91" s="10">
+      <c r="E91" s="9">
         <v>1663.96</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="7">
+      <c r="B92" s="6">
         <v>670</v>
       </c>
-      <c r="C92" s="9">
+      <c r="C92" s="8">
         <v>3359.32</v>
       </c>
-      <c r="D92" s="9">
+      <c r="D92" s="8">
         <f t="shared" si="1"/>
         <v>335.93200000000002</v>
       </c>
-      <c r="E92" s="10">
+      <c r="E92" s="9">
         <v>1679.66</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="7">
+      <c r="B93" s="6">
         <v>680</v>
       </c>
-      <c r="C93" s="9">
+      <c r="C93" s="8">
         <v>3390.61</v>
       </c>
-      <c r="D93" s="9">
+      <c r="D93" s="8">
         <f t="shared" si="1"/>
         <v>339.06100000000004</v>
       </c>
-      <c r="E93" s="10">
+      <c r="E93" s="9">
         <v>1695.3</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="7">
+      <c r="B94" s="6">
         <v>690</v>
       </c>
-      <c r="C94" s="9">
+      <c r="C94" s="8">
         <v>3421.78</v>
       </c>
-      <c r="D94" s="9">
+      <c r="D94" s="8">
         <f t="shared" si="1"/>
         <v>342.178</v>
       </c>
-      <c r="E94" s="10">
+      <c r="E94" s="9">
         <v>1710.89</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B95" s="7">
+      <c r="B95" s="6">
         <v>700</v>
       </c>
-      <c r="C95" s="9">
+      <c r="C95" s="8">
         <v>3452.84</v>
       </c>
-      <c r="D95" s="9">
+      <c r="D95" s="8">
         <f t="shared" si="1"/>
         <v>345.28399999999999</v>
       </c>
-      <c r="E95" s="10">
+      <c r="E95" s="9">
         <v>1726.42</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="7">
+      <c r="B96" s="6">
         <v>710</v>
       </c>
-      <c r="C96" s="9">
+      <c r="C96" s="8">
         <v>3483.78</v>
       </c>
-      <c r="D96" s="9">
+      <c r="D96" s="8">
         <f t="shared" si="1"/>
         <v>348.37800000000004</v>
       </c>
-      <c r="E96" s="10">
+      <c r="E96" s="9">
         <v>1741.89</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B97" s="7">
+      <c r="B97" s="6">
         <v>720</v>
       </c>
-      <c r="C97" s="9">
+      <c r="C97" s="8">
         <v>3514.6</v>
       </c>
-      <c r="D97" s="9">
+      <c r="D97" s="8">
         <f t="shared" si="1"/>
         <v>351.46</v>
       </c>
-      <c r="E97" s="10">
+      <c r="E97" s="9">
         <v>1757.3</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B98" s="7">
+      <c r="B98" s="6">
         <v>730</v>
       </c>
-      <c r="C98" s="9">
+      <c r="C98" s="8">
         <v>3545.31</v>
       </c>
-      <c r="D98" s="9">
+      <c r="D98" s="8">
         <f t="shared" si="1"/>
         <v>354.53100000000001</v>
       </c>
-      <c r="E98" s="10">
+      <c r="E98" s="9">
         <v>1772.65</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B99" s="7">
+      <c r="B99" s="6">
         <v>740</v>
       </c>
-      <c r="C99" s="9">
+      <c r="C99" s="8">
         <v>3575.9</v>
       </c>
-      <c r="D99" s="9">
+      <c r="D99" s="8">
         <f t="shared" si="1"/>
         <v>357.59000000000003</v>
       </c>
-      <c r="E99" s="10">
+      <c r="E99" s="9">
         <v>1787.95</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B100" s="7">
+      <c r="B100" s="6">
         <v>750</v>
       </c>
-      <c r="C100" s="9">
+      <c r="C100" s="8">
         <v>3606.38</v>
       </c>
-      <c r="D100" s="9">
+      <c r="D100" s="8">
         <f t="shared" si="1"/>
         <v>360.63800000000003</v>
       </c>
-      <c r="E100" s="10">
+      <c r="E100" s="9">
         <v>1803.19</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B101" s="7">
+      <c r="B101" s="6">
         <v>760</v>
       </c>
-      <c r="C101" s="9">
+      <c r="C101" s="8">
         <v>3636.74</v>
       </c>
-      <c r="D101" s="9">
+      <c r="D101" s="8">
         <f t="shared" si="1"/>
         <v>363.67399999999998</v>
       </c>
-      <c r="E101" s="10">
+      <c r="E101" s="9">
         <v>1818.37</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="7">
+      <c r="B102" s="6">
         <v>770</v>
       </c>
-      <c r="C102" s="9">
+      <c r="C102" s="8">
         <v>3666.99</v>
       </c>
-      <c r="D102" s="9">
+      <c r="D102" s="8">
         <f t="shared" si="1"/>
         <v>366.69899999999996</v>
       </c>
-      <c r="E102" s="10">
+      <c r="E102" s="9">
         <v>1833.5</v>
       </c>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B103" s="7">
+      <c r="B103" s="6">
         <v>780</v>
       </c>
-      <c r="C103" s="9">
+      <c r="C103" s="8">
         <v>3697.12</v>
       </c>
-      <c r="D103" s="9">
+      <c r="D103" s="8">
         <f t="shared" si="1"/>
         <v>369.71199999999999</v>
       </c>
-      <c r="E103" s="10">
+      <c r="E103" s="9">
         <v>1848.56</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B104" s="7">
+      <c r="B104" s="6">
         <v>790</v>
       </c>
-      <c r="C104" s="9">
+      <c r="C104" s="8">
         <v>3727.14</v>
       </c>
-      <c r="D104" s="9">
+      <c r="D104" s="8">
         <f t="shared" si="1"/>
         <v>372.714</v>
       </c>
-      <c r="E104" s="10">
+      <c r="E104" s="9">
         <v>1863.57</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B105" s="7">
+      <c r="B105" s="6">
         <v>800</v>
       </c>
-      <c r="C105" s="9">
+      <c r="C105" s="8">
         <v>3757.04</v>
       </c>
-      <c r="D105" s="9">
+      <c r="D105" s="8">
         <f t="shared" si="1"/>
         <v>375.70400000000001</v>
       </c>
-      <c r="E105" s="10">
+      <c r="E105" s="9">
         <v>1878.52</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B106" s="7">
+      <c r="B106" s="6">
         <v>810</v>
       </c>
-      <c r="C106" s="9">
+      <c r="C106" s="8">
         <v>3786.83</v>
       </c>
-      <c r="D106" s="9">
+      <c r="D106" s="8">
         <f t="shared" si="1"/>
         <v>378.68299999999999</v>
       </c>
-      <c r="E106" s="10">
+      <c r="E106" s="9">
         <v>1893.41</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B107" s="7">
+      <c r="B107" s="6">
         <v>820</v>
       </c>
-      <c r="C107" s="9">
+      <c r="C107" s="8">
         <v>3816.5</v>
       </c>
-      <c r="D107" s="9">
+      <c r="D107" s="8">
         <f t="shared" si="1"/>
         <v>381.65</v>
       </c>
-      <c r="E107" s="10">
+      <c r="E107" s="9">
         <v>1908.25</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B108" s="7">
+      <c r="B108" s="6">
         <v>830</v>
       </c>
-      <c r="C108" s="9">
+      <c r="C108" s="8">
         <v>3846.05</v>
       </c>
-      <c r="D108" s="9">
+      <c r="D108" s="8">
         <f t="shared" si="1"/>
         <v>384.60500000000002</v>
       </c>
-      <c r="E108" s="10">
+      <c r="E108" s="9">
         <v>1923.02</v>
       </c>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B109" s="7">
+      <c r="B109" s="6">
         <v>840</v>
       </c>
-      <c r="C109" s="9">
+      <c r="C109" s="8">
         <v>3875.49</v>
       </c>
-      <c r="D109" s="9">
+      <c r="D109" s="8">
         <f t="shared" si="1"/>
         <v>387.54899999999998</v>
       </c>
-      <c r="E109" s="10">
+      <c r="E109" s="9">
         <v>1937.74</v>
       </c>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B110" s="7">
+      <c r="B110" s="6">
         <v>850</v>
       </c>
-      <c r="C110" s="9">
+      <c r="C110" s="8">
         <v>3904.81</v>
       </c>
-      <c r="D110" s="9">
+      <c r="D110" s="8">
         <f t="shared" si="1"/>
         <v>390.48099999999999</v>
       </c>
-      <c r="E110" s="15"/>
+      <c r="E110" s="14"/>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C111" s="6"/>
+      <c r="C111" s="5"/>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C112" s="6"/>
+      <c r="C112" s="5"/>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C113" s="6"/>
+      <c r="C113" s="5"/>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C114" s="6"/>
+      <c r="C114" s="5"/>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C115" s="6"/>
+      <c r="C115" s="5"/>
     </row>
     <row r="116" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C116" s="6"/>
+      <c r="C116" s="5"/>
     </row>
     <row r="117" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C117" s="6"/>
+      <c r="C117" s="5"/>
     </row>
     <row r="118" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C118" s="6"/>
+      <c r="C118" s="5"/>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C119" s="6"/>
+      <c r="C119" s="5"/>
     </row>
     <row r="120" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C120" s="6"/>
+      <c r="C120" s="5"/>
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C121" s="6"/>
+      <c r="C121" s="5"/>
     </row>
     <row r="122" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C122" s="6"/>
+      <c r="C122" s="5"/>
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C123" s="6"/>
+      <c r="C123" s="5"/>
     </row>
     <row r="124" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C124" s="6"/>
+      <c r="C124" s="5"/>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C125" s="6"/>
+      <c r="C125" s="5"/>
     </row>
     <row r="126" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C126" s="6"/>
+      <c r="C126" s="5"/>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C127" s="6"/>
+      <c r="C127" s="5"/>
     </row>
     <row r="128" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C128" s="6"/>
+      <c r="C128" s="5"/>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C129" s="6"/>
+      <c r="C129" s="5"/>
     </row>
     <row r="130" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C130" s="6"/>
+      <c r="C130" s="5"/>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C131" s="6"/>
+      <c r="C131" s="5"/>
     </row>
     <row r="132" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C132" s="6"/>
+      <c r="C132" s="5"/>
     </row>
     <row r="133" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C133" s="6"/>
+      <c r="C133" s="5"/>
     </row>
     <row r="134" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C134" s="6"/>
+      <c r="C134" s="5"/>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C135" s="6"/>
+      <c r="C135" s="5"/>
     </row>
     <row r="136" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C136" s="6"/>
+      <c r="C136" s="5"/>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C137" s="6"/>
+      <c r="C137" s="5"/>
     </row>
     <row r="138" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C138" s="6"/>
+      <c r="C138" s="5"/>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C139" s="6"/>
+      <c r="C139" s="5"/>
     </row>
     <row r="140" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C140" s="6"/>
+      <c r="C140" s="5"/>
     </row>
     <row r="141" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C141" s="6"/>
+      <c r="C141" s="5"/>
     </row>
     <row r="142" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C142" s="6"/>
+      <c r="C142" s="5"/>
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C143" s="6"/>
+      <c r="C143" s="5"/>
     </row>
     <row r="144" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C144" s="6"/>
+      <c r="C144" s="5"/>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C145" s="6"/>
+      <c r="C145" s="5"/>
     </row>
     <row r="146" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C146" s="6"/>
+      <c r="C146" s="5"/>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C147" s="6"/>
+      <c r="C147" s="5"/>
     </row>
     <row r="148" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C148" s="6"/>
+      <c r="C148" s="5"/>
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C149" s="6"/>
+      <c r="C149" s="5"/>
     </row>
     <row r="150" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C150" s="6"/>
+      <c r="C150" s="5"/>
     </row>
     <row r="151" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C151" s="6"/>
+      <c r="C151" s="5"/>
     </row>
     <row r="152" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C152" s="6"/>
+      <c r="C152" s="5"/>
     </row>
     <row r="153" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C153" s="6"/>
+      <c r="C153" s="5"/>
     </row>
     <row r="154" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C154" s="6"/>
+      <c r="C154" s="5"/>
     </row>
     <row r="155" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C155" s="6"/>
+      <c r="C155" s="5"/>
     </row>
     <row r="156" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C156" s="6"/>
+      <c r="C156" s="5"/>
     </row>
     <row r="157" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C157" s="6"/>
+      <c r="C157" s="5"/>
     </row>
     <row r="158" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C158" s="6"/>
+      <c r="C158" s="5"/>
     </row>
     <row r="159" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C159" s="6"/>
+      <c r="C159" s="5"/>
     </row>
     <row r="160" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C160" s="6"/>
+      <c r="C160" s="5"/>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C161" s="6"/>
+      <c r="C161" s="5"/>
     </row>
     <row r="162" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C162" s="6"/>
+      <c r="C162" s="5"/>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C163" s="6"/>
+      <c r="C163" s="5"/>
     </row>
     <row r="164" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C164" s="6"/>
+      <c r="C164" s="5"/>
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C165" s="6"/>
+      <c r="C165" s="5"/>
     </row>
     <row r="166" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C166" s="6"/>
+      <c r="C166" s="5"/>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C167" s="6"/>
+      <c r="C167" s="5"/>
     </row>
     <row r="168" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C168" s="6"/>
+      <c r="C168" s="5"/>
     </row>
     <row r="169" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C169" s="6"/>
+      <c r="C169" s="5"/>
     </row>
     <row r="170" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C170" s="6"/>
+      <c r="C170" s="5"/>
     </row>
     <row r="171" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C171" s="6"/>
+      <c r="C171" s="5"/>
     </row>
     <row r="172" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C172" s="6"/>
+      <c r="C172" s="5"/>
     </row>
     <row r="173" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C173" s="6"/>
+      <c r="C173" s="5"/>
     </row>
     <row r="174" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C174" s="6"/>
+      <c r="C174" s="5"/>
     </row>
     <row r="175" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C175" s="6"/>
+      <c r="C175" s="5"/>
     </row>
     <row r="176" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C176" s="6"/>
+      <c r="C176" s="5"/>
     </row>
     <row r="177" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C177" s="6"/>
+      <c r="C177" s="5"/>
     </row>
     <row r="178" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C178" s="6"/>
+      <c r="C178" s="5"/>
     </row>
     <row r="179" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C179" s="6"/>
+      <c r="C179" s="5"/>
     </row>
     <row r="180" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C180" s="6"/>
+      <c r="C180" s="5"/>
     </row>
     <row r="181" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C181" s="6"/>
+      <c r="C181" s="5"/>
     </row>
     <row r="182" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C182" s="6"/>
+      <c r="C182" s="5"/>
     </row>
     <row r="183" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C183" s="6"/>
+      <c r="C183" s="5"/>
     </row>
     <row r="184" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C184" s="6"/>
+      <c r="C184" s="5"/>
     </row>
     <row r="185" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C185" s="6"/>
+      <c r="C185" s="5"/>
     </row>
     <row r="186" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C186" s="6"/>
+      <c r="C186" s="5"/>
     </row>
     <row r="187" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C187" s="6"/>
+      <c r="C187" s="5"/>
     </row>
     <row r="188" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C188" s="6"/>
+      <c r="C188" s="5"/>
     </row>
     <row r="189" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C189" s="6"/>
+      <c r="C189" s="5"/>
     </row>
     <row r="190" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C190" s="6"/>
+      <c r="C190" s="5"/>
     </row>
     <row r="191" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C191" s="6"/>
+      <c r="C191" s="5"/>
     </row>
     <row r="192" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C192" s="6"/>
+      <c r="C192" s="5"/>
     </row>
     <row r="193" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C193" s="6"/>
+      <c r="C193" s="5"/>
     </row>
     <row r="194" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C194" s="6"/>
+      <c r="C194" s="5"/>
     </row>
     <row r="195" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C195" s="6"/>
+      <c r="C195" s="5"/>
     </row>
     <row r="196" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C196" s="6"/>
+      <c r="C196" s="5"/>
     </row>
     <row r="197" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C197" s="6"/>
+      <c r="C197" s="5"/>
     </row>
     <row r="198" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C198" s="6"/>
+      <c r="C198" s="5"/>
     </row>
     <row r="199" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C199" s="6"/>
+      <c r="C199" s="5"/>
     </row>
     <row r="200" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C200" s="6"/>
+      <c r="C200" s="5"/>
     </row>
     <row r="201" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C201" s="6"/>
+      <c r="C201" s="5"/>
     </row>
     <row r="202" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C202" s="6"/>
+      <c r="C202" s="5"/>
     </row>
     <row r="203" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C203" s="6"/>
+      <c r="C203" s="5"/>
     </row>
     <row r="204" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C204" s="6"/>
+      <c r="C204" s="5"/>
     </row>
     <row r="205" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C205" s="6"/>
+      <c r="C205" s="5"/>
     </row>
     <row r="206" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C206" s="6"/>
+      <c r="C206" s="5"/>
     </row>
     <row r="207" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C207" s="6"/>
+      <c r="C207" s="5"/>
     </row>
     <row r="208" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C208" s="6"/>
+      <c r="C208" s="5"/>
     </row>
     <row r="209" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C209" s="6"/>
+      <c r="C209" s="5"/>
     </row>
     <row r="210" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C210" s="6"/>
+      <c r="C210" s="5"/>
     </row>
     <row r="211" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C211" s="6"/>
+      <c r="C211" s="5"/>
     </row>
     <row r="212" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C212" s="6"/>
+      <c r="C212" s="5"/>
     </row>
     <row r="213" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C213" s="6"/>
+      <c r="C213" s="5"/>
     </row>
     <row r="214" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C214" s="6"/>
+      <c r="C214" s="5"/>
     </row>
     <row r="215" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C215" s="6"/>
+      <c r="C215" s="5"/>
     </row>
     <row r="216" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C216" s="6"/>
+      <c r="C216" s="5"/>
     </row>
     <row r="217" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C217" s="6"/>
+      <c r="C217" s="5"/>
     </row>
     <row r="218" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C218" s="6"/>
+      <c r="C218" s="5"/>
     </row>
     <row r="219" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C219" s="6"/>
+      <c r="C219" s="5"/>
     </row>
     <row r="220" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C220" s="6"/>
+      <c r="C220" s="5"/>
     </row>
     <row r="221" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C221" s="6"/>
+      <c r="C221" s="5"/>
     </row>
     <row r="222" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C222" s="6"/>
+      <c r="C222" s="5"/>
     </row>
     <row r="223" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C223" s="6"/>
+      <c r="C223" s="5"/>
     </row>
     <row r="224" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C224" s="6"/>
+      <c r="C224" s="5"/>
     </row>
     <row r="225" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C225" s="6"/>
+      <c r="C225" s="5"/>
     </row>
     <row r="226" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C226" s="6"/>
+      <c r="C226" s="5"/>
     </row>
     <row r="227" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C227" s="6"/>
+      <c r="C227" s="5"/>
     </row>
     <row r="228" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C228" s="6"/>
+      <c r="C228" s="5"/>
     </row>
     <row r="229" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C229" s="6"/>
+      <c r="C229" s="5"/>
     </row>
     <row r="230" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C230" s="6"/>
+      <c r="C230" s="5"/>
     </row>
     <row r="231" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C231" s="6"/>
+      <c r="C231" s="5"/>
     </row>
     <row r="232" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C232" s="6"/>
+      <c r="C232" s="5"/>
     </row>
     <row r="233" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C233" s="6"/>
+      <c r="C233" s="5"/>
     </row>
     <row r="234" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C234" s="6"/>
+      <c r="C234" s="5"/>
     </row>
     <row r="235" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C235" s="6"/>
+      <c r="C235" s="5"/>
     </row>
     <row r="236" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C236" s="6"/>
+      <c r="C236" s="5"/>
     </row>
     <row r="237" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C237" s="6"/>
+      <c r="C237" s="5"/>
     </row>
     <row r="238" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C238" s="6"/>
+      <c r="C238" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
- removed pic - updated table
</commit_message>
<xml_diff>
--- a/doc/pt1000_pt100_pt500_tables.xlsx
+++ b/doc/pt1000_pt100_pt500_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_SELTRON\zigamiklosic\Personal\HomeWork\RND_Thermal_Modeling\src\drivers\devices\thermistor\thermistor\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DB5868-0114-4F14-B50F-009693423D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0567D9E4-7DB9-4C60-A9EF-40C14D84349F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3039,7 +3039,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4000"/>
-          <c:min val="-10"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4125,7 +4125,7 @@
   <dimension ref="B1:AD238"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R49" sqref="R49"/>
+      <selection activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- updated changelog - updated excel file
</commit_message>
<xml_diff>
--- a/doc/pt1000_pt100_pt500_tables.xlsx
+++ b/doc/pt1000_pt100_pt500_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tinkara.marcec\Downloads\thermistor-develop\thermistor-develop\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_SELTRON\zigamiklosic\Personal\HomeWork\RND_Thermal_Modeling\src\drivers\devices\thermistor\thermistor\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D0CA0C-9F09-4FCE-9EB0-307557ADBB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF0D916-B9A2-4A92-941E-44DAC61E234A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PT Values" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>PT100 [Ohm]</t>
   </si>
@@ -225,9 +225,6 @@
   <si>
     <t>n/a</t>
   </si>
-  <si>
-    <t>¸¸</t>
-  </si>
 </sst>
 </file>
 
@@ -321,7 +318,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +328,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,56 +543,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -599,6 +557,51 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,7 +715,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'PT Values'!$C$9</c:f>
+              <c:f>'PT Values'!$C$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -775,7 +778,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'PT Values'!$B$10:$B$115</c:f>
+              <c:f>'PT Values'!$B$11:$B$116</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="106"/>
@@ -1102,7 +1105,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PT Values'!$C$10:$C$115</c:f>
+              <c:f>'PT Values'!$C$11:$C$116</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="106"/>
@@ -1439,7 +1442,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'PT Values'!$D$9</c:f>
+              <c:f>'PT Values'!$D$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1474,7 +1477,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'PT Values'!$B$10:$B$115</c:f>
+              <c:f>'PT Values'!$B$11:$B$116</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="106"/>
@@ -1801,7 +1804,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PT Values'!$D$10:$D$115</c:f>
+              <c:f>'PT Values'!$D$11:$D$116</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="106"/>
@@ -2138,7 +2141,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'PT Values'!$E$9</c:f>
+              <c:f>'PT Values'!$E$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2173,7 +2176,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'PT Values'!$B$10:$B$115</c:f>
+              <c:f>'PT Values'!$B$11:$B$116</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="106"/>
@@ -2500,7 +2503,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PT Values'!$E$10:$E$115</c:f>
+              <c:f>'PT Values'!$E$11:$E$116</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="106"/>
@@ -3301,7 +3304,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'PT Values'!$B$10:$B$115</c:f>
+              <c:f>'PT Values'!$B$11:$B$116</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="106"/>
@@ -3628,7 +3631,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PT Values'!$I$10:$I$115</c:f>
+              <c:f>'PT Values'!$I$11:$I$116</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="106"/>
@@ -5391,13 +5394,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>272143</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>32964</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>583500</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>142503</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5427,13 +5430,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>258536</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>138792</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5725,10 +5728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AD243"/>
+  <dimension ref="B1:AD244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5743,58 +5746,41 @@
     <col min="9" max="9" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:30" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:13" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="28"/>
-    </row>
-    <row r="2" spans="2:30" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="31"/>
-    </row>
-    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-    </row>
-    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19" t="s">
-        <v>11</v>
-      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="24"/>
+    </row>
+    <row r="3" spans="2:13" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="27"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -5805,15 +5791,13 @@
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
     </row>
-    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="21">
-        <v>3.9083E-3</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>10</v>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -5825,16 +5809,15 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="24">
-        <f>-5.775*10^-7</f>
-        <v>-5.7749999999999998E-7</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>9</v>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="29">
+        <v>3.9083E-3</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>10</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
@@ -5846,10 +5829,17 @@
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
     </row>
-    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="32">
+        <f>-5.775*10^-7</f>
+        <v>-5.7749999999999998E-7</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>9</v>
+      </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
@@ -5860,2911 +5850,2919 @@
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="2:30" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+    </row>
+    <row r="9" spans="2:13" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="32" t="s">
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="2:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C10" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I10" s="19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
         <v>-200</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C11" s="7">
         <v>185.2</v>
       </c>
-      <c r="D10" s="8">
-        <f>C10/10</f>
+      <c r="D11" s="8">
+        <f>C11/10</f>
         <v>18.52</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="G10" s="35">
-        <f>(-$C$5+SQRT($C$5*$C$5-4*$C$6*(1-C10/1000)))/(2*$C$6)</f>
+      <c r="E11" s="13"/>
+      <c r="G11" s="20">
+        <f>(-$C$6+SQRT($C$6*$C$6-4*$C$7*(1-C11/1000)))/(2*$C$7)</f>
         <v>-202.4247106393542</v>
       </c>
-      <c r="H10" s="35">
-        <f>B10-G10</f>
+      <c r="H11" s="20">
+        <f>B11-G11</f>
         <v>2.4247106393542026</v>
       </c>
-      <c r="I10" s="35">
-        <f>H10/B10*100</f>
+      <c r="I11" s="20">
+        <f>H11/B11*100</f>
         <v>-1.2123553196771013</v>
       </c>
-      <c r="K10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
         <v>-190</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C12" s="7">
         <v>228.25</v>
       </c>
-      <c r="D11" s="8">
-        <f t="shared" ref="D11:D74" si="0">C11/10</f>
+      <c r="D12" s="8">
+        <f t="shared" ref="D12:D75" si="0">C12/10</f>
         <v>22.824999999999999</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E12" s="9">
         <v>114.13</v>
       </c>
-      <c r="G11" s="35">
-        <f t="shared" ref="G11:G74" si="1">(-$C$5+SQRT($C$5*$C$5-4*$C$6*(1-C11/1000)))/(2*$C$6)</f>
+      <c r="G12" s="20">
+        <f t="shared" ref="G12:G75" si="1">(-$C$6+SQRT($C$6*$C$6-4*$C$7*(1-C12/1000)))/(2*$C$7)</f>
         <v>-192.01632902331164</v>
       </c>
-      <c r="H11" s="35">
-        <f t="shared" ref="H11:H74" si="2">B11-G11</f>
+      <c r="H12" s="20">
+        <f t="shared" ref="H12:H75" si="2">B12-G12</f>
         <v>2.0163290233116413</v>
       </c>
-      <c r="I11" s="35">
-        <f t="shared" ref="I11:I74" si="3">H11/B11*100</f>
+      <c r="I12" s="20">
+        <f t="shared" ref="I12:I75" si="3">H12/B12*100</f>
         <v>-1.061225801742969</v>
       </c>
     </row>
-    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
         <v>-180</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C13" s="7">
         <v>270.95999999999998</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D13" s="8">
         <f t="shared" si="0"/>
         <v>27.095999999999997</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E13" s="9">
         <v>135.47999999999999</v>
       </c>
-      <c r="G12" s="35">
+      <c r="G13" s="20">
         <f t="shared" si="1"/>
         <v>-181.66012545562819</v>
       </c>
-      <c r="H12" s="35">
+      <c r="H13" s="20">
         <f t="shared" si="2"/>
         <v>1.6601254556281901</v>
       </c>
-      <c r="I12" s="35">
+      <c r="I13" s="20">
         <f t="shared" si="3"/>
         <v>-0.92229191979343894</v>
       </c>
     </row>
-    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
         <v>-170</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C14" s="7">
         <v>313.35000000000002</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D14" s="8">
         <f t="shared" si="0"/>
         <v>31.335000000000001</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E14" s="9">
         <v>156.68</v>
       </c>
-      <c r="G13" s="35">
+      <c r="G14" s="20">
         <f t="shared" si="1"/>
         <v>-171.35168525376764</v>
       </c>
-      <c r="H13" s="35">
+      <c r="H14" s="20">
         <f t="shared" si="2"/>
         <v>1.3516852537676414</v>
       </c>
-      <c r="I13" s="35">
+      <c r="I14" s="20">
         <f t="shared" si="3"/>
         <v>-0.79510897280449488</v>
       </c>
     </row>
-    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
         <v>-160</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C15" s="7">
         <v>355.45</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D15" s="8">
         <f t="shared" si="0"/>
         <v>35.545000000000002</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E15" s="9">
         <v>177.72</v>
       </c>
-      <c r="G14" s="35">
+      <c r="G15" s="20">
         <f t="shared" si="1"/>
         <v>-161.08409794105449</v>
       </c>
-      <c r="H14" s="35">
+      <c r="H15" s="20">
         <f t="shared" si="2"/>
         <v>1.0840979410544946</v>
       </c>
-      <c r="I14" s="35">
+      <c r="I15" s="20">
         <f t="shared" si="3"/>
         <v>-0.67756121315905915</v>
       </c>
     </row>
-    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
         <v>-150</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C16" s="7">
         <v>397.23</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D16" s="8">
         <f t="shared" si="0"/>
         <v>39.722999999999999</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E16" s="9">
         <v>198.62</v>
       </c>
-      <c r="G15" s="35">
+      <c r="G16" s="20">
         <f t="shared" si="1"/>
         <v>-150.86506788652258</v>
       </c>
-      <c r="H15" s="35">
+      <c r="H16" s="20">
         <f t="shared" si="2"/>
         <v>0.86506788652258138</v>
       </c>
-      <c r="I15" s="35">
+      <c r="I16" s="20">
         <f t="shared" si="3"/>
         <v>-0.57671192434838758</v>
       </c>
     </row>
-    <row r="16" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="6">
+    <row r="17" spans="2:30" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="6">
         <v>-140</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C17" s="7">
         <v>438.76</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D17" s="8">
         <f t="shared" si="0"/>
         <v>43.875999999999998</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E17" s="9">
         <v>219.38</v>
       </c>
-      <c r="G16" s="35">
+      <c r="G17" s="20">
         <f t="shared" si="1"/>
         <v>-140.67782178673895</v>
       </c>
-      <c r="H16" s="35">
+      <c r="H17" s="20">
         <f t="shared" si="2"/>
         <v>0.67782178673894578</v>
       </c>
-      <c r="I16" s="35">
+      <c r="I17" s="20">
         <f t="shared" si="3"/>
         <v>-0.48415841909924695</v>
       </c>
-      <c r="AD16" s="14"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
+      <c r="AD17" s="14"/>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
         <v>-130</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C18" s="7">
         <v>480.05</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D18" s="8">
         <f t="shared" si="0"/>
         <v>48.005000000000003</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E18" s="9">
         <v>240.02</v>
       </c>
-      <c r="G17" s="35">
+      <c r="G18" s="20">
         <f t="shared" si="1"/>
         <v>-130.52017241568328</v>
       </c>
-      <c r="H17" s="35">
+      <c r="H18" s="20">
         <f t="shared" si="2"/>
         <v>0.52017241568327677</v>
       </c>
-      <c r="I17" s="35">
+      <c r="I18" s="20">
         <f t="shared" si="3"/>
         <v>-0.40013262744867445</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="6">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
         <v>-120</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C19" s="7">
         <v>521.1</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D19" s="8">
         <f t="shared" si="0"/>
         <v>52.11</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E19" s="9">
         <v>260.55</v>
       </c>
-      <c r="G18" s="35">
+      <c r="G19" s="20">
         <f t="shared" si="1"/>
         <v>-120.39237714996712</v>
       </c>
-      <c r="H18" s="35">
+      <c r="H19" s="20">
         <f t="shared" si="2"/>
         <v>0.39237714996711759</v>
       </c>
-      <c r="I18" s="35">
+      <c r="I19" s="20">
         <f t="shared" si="3"/>
         <v>-0.32698095830593132</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="6">
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
         <v>-110</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C20" s="7">
         <v>561.92999999999995</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D20" s="8">
         <f t="shared" si="0"/>
         <v>56.192999999999998</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E20" s="9">
         <v>280.97000000000003</v>
       </c>
-      <c r="G19" s="35">
+      <c r="G20" s="20">
         <f t="shared" si="1"/>
         <v>-110.28973980432009</v>
       </c>
-      <c r="H19" s="35">
+      <c r="H20" s="20">
         <f t="shared" si="2"/>
         <v>0.28973980432009228</v>
       </c>
-      <c r="I19" s="35">
+      <c r="I20" s="20">
         <f t="shared" si="3"/>
         <v>-0.26339982210917479</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="6">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
         <v>-100</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C21" s="7">
         <v>602.55999999999995</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D21" s="8">
         <f t="shared" si="0"/>
         <v>60.255999999999993</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E21" s="9">
         <v>301.27999999999997</v>
       </c>
-      <c r="G20" s="35">
+      <c r="G21" s="20">
         <f t="shared" si="1"/>
         <v>-100.20750910403933</v>
       </c>
-      <c r="H20" s="35">
+      <c r="H21" s="20">
         <f t="shared" si="2"/>
         <v>0.20750910403933176</v>
       </c>
-      <c r="I20" s="35">
+      <c r="I21" s="20">
         <f t="shared" si="3"/>
         <v>-0.20750910403933173</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="6">
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
         <v>-90</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C22" s="7">
         <v>643</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D22" s="8">
         <f t="shared" si="0"/>
         <v>64.3</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E22" s="9">
         <v>321.5</v>
       </c>
-      <c r="G21" s="35">
+      <c r="G22" s="20">
         <f t="shared" si="1"/>
         <v>-90.143370460324178</v>
       </c>
-      <c r="H21" s="35">
+      <c r="H22" s="20">
         <f t="shared" si="2"/>
         <v>0.14337046032417788</v>
       </c>
-      <c r="I21" s="35">
+      <c r="I22" s="20">
         <f t="shared" si="3"/>
         <v>-0.15930051147130875</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="6">
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
         <v>-80</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C23" s="7">
         <v>683.25</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D23" s="8">
         <f t="shared" si="0"/>
         <v>68.325000000000003</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E23" s="9">
         <v>341.63</v>
       </c>
-      <c r="G22" s="35">
+      <c r="G23" s="20">
         <f t="shared" si="1"/>
         <v>-80.097481568779955</v>
       </c>
-      <c r="H22" s="35">
+      <c r="H23" s="20">
         <f t="shared" si="2"/>
         <v>9.7481568779954841E-2</v>
       </c>
-      <c r="I22" s="35">
+      <c r="I23" s="20">
         <f t="shared" si="3"/>
         <v>-0.12185196097494355</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="6">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
         <v>-70</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C24" s="7">
         <v>723.35</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D24" s="8">
         <f t="shared" si="0"/>
         <v>72.335000000000008</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E24" s="9">
         <v>361.67</v>
       </c>
-      <c r="G23" s="35">
+      <c r="G24" s="20">
         <f t="shared" si="1"/>
         <v>-70.059974661959927</v>
       </c>
-      <c r="H23" s="35">
+      <c r="H24" s="20">
         <f t="shared" si="2"/>
         <v>5.9974661959927289E-2</v>
       </c>
-      <c r="I23" s="35">
+      <c r="I24" s="20">
         <f t="shared" si="3"/>
         <v>-8.5678088514181835E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="6">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
         <v>-60</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C25" s="7">
         <v>763.28</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D25" s="8">
         <f t="shared" si="0"/>
         <v>76.328000000000003</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E25" s="9">
         <v>381.64</v>
       </c>
-      <c r="G24" s="35">
+      <c r="G25" s="20">
         <f t="shared" si="1"/>
         <v>-60.035951139780046</v>
       </c>
-      <c r="H24" s="35">
+      <c r="H25" s="20">
         <f t="shared" si="2"/>
         <v>3.5951139780046049E-2</v>
       </c>
-      <c r="I24" s="35">
+      <c r="I25" s="20">
         <f t="shared" si="3"/>
         <v>-5.9918566300076748E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="6">
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
         <v>-50</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C26" s="7">
         <v>803.06</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D26" s="8">
         <f t="shared" si="0"/>
         <v>80.305999999999997</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E26" s="9">
         <v>401.53</v>
       </c>
-      <c r="G25" s="35">
+      <c r="G26" s="20">
         <f t="shared" si="1"/>
         <v>-50.020486317023334</v>
       </c>
-      <c r="H25" s="35">
+      <c r="H26" s="20">
         <f t="shared" si="2"/>
         <v>2.0486317023333811E-2</v>
       </c>
-      <c r="I25" s="35">
+      <c r="I26" s="20">
         <f t="shared" si="3"/>
         <v>-4.0972634046667622E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="6">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
         <v>-40</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C27" s="7">
         <v>842.71</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D27" s="8">
         <f t="shared" si="0"/>
         <v>84.271000000000001</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E27" s="9">
         <v>421.35</v>
       </c>
-      <c r="G26" s="35">
+      <c r="G27" s="20">
         <f t="shared" si="1"/>
         <v>-40.008597789179348</v>
       </c>
-      <c r="H26" s="35">
+      <c r="H27" s="20">
         <f t="shared" si="2"/>
         <v>8.5977891793476147E-3</v>
       </c>
-      <c r="I26" s="35">
+      <c r="I27" s="20">
         <f t="shared" si="3"/>
         <v>-2.1494472948369037E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="6">
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
         <v>-30</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C28" s="7">
         <v>882.22</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D28" s="8">
         <f t="shared" si="0"/>
         <v>88.222000000000008</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E28" s="9">
         <v>441.11</v>
       </c>
-      <c r="G27" s="35">
+      <c r="G28" s="20">
         <f t="shared" si="1"/>
         <v>-30.002853192482927</v>
       </c>
-      <c r="H27" s="35">
+      <c r="H28" s="20">
         <f t="shared" si="2"/>
         <v>2.8531924829273692E-3</v>
       </c>
-      <c r="I27" s="35">
+      <c r="I28" s="20">
         <f t="shared" si="3"/>
         <v>-9.5106416097578972E-3</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="6">
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
         <v>-20</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C29" s="9">
         <v>921.6</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D29" s="8">
         <f t="shared" si="0"/>
         <v>92.16</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E29" s="9">
         <v>460.8</v>
       </c>
-      <c r="G28" s="35">
+      <c r="G29" s="20">
         <f t="shared" si="1"/>
         <v>-20.000763086855635</v>
       </c>
-      <c r="H28" s="35">
+      <c r="H29" s="20">
         <f t="shared" si="2"/>
         <v>7.6308685563475365E-4</v>
       </c>
-      <c r="I28" s="35">
+      <c r="I29" s="20">
         <f t="shared" si="3"/>
         <v>-3.8154342781737682E-3</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="6">
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B30" s="6">
         <v>-10</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C30" s="9">
         <v>960.86</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D30" s="8">
         <f t="shared" si="0"/>
         <v>96.085999999999999</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E30" s="9">
         <v>480.43</v>
       </c>
-      <c r="G29" s="35">
+      <c r="G30" s="20">
         <f t="shared" si="1"/>
         <v>-9.9998086661426608</v>
       </c>
-      <c r="H29" s="35">
+      <c r="H30" s="20">
         <f t="shared" si="2"/>
         <v>-1.9133385733915986E-4</v>
       </c>
-      <c r="I29" s="35">
+      <c r="I30" s="20">
         <f t="shared" si="3"/>
         <v>1.9133385733915988E-3</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="6">
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
         <v>0</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C31" s="9">
         <v>1000</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D31" s="8">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E31" s="9">
         <v>500</v>
       </c>
-      <c r="G30" s="35">
+      <c r="G31" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H30" s="35">
+      <c r="H31" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I30" s="35" t="s">
+      <c r="I31" s="20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="6">
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B32" s="6">
         <v>10</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C32" s="9">
         <v>1039.03</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D32" s="8">
         <f t="shared" si="0"/>
         <v>103.90299999999999</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E32" s="9">
         <v>519.51</v>
       </c>
-      <c r="G31" s="35">
+      <c r="G32" s="20">
         <f t="shared" si="1"/>
         <v>10.001218964741643</v>
       </c>
-      <c r="H31" s="35">
+      <c r="H32" s="20">
         <f t="shared" si="2"/>
         <v>-1.2189647416427363E-3</v>
       </c>
-      <c r="I31" s="35">
+      <c r="I32" s="20">
         <f t="shared" si="3"/>
         <v>-1.2189647416427363E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="6">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
         <v>20</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C33" s="9">
         <v>1077.94</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D33" s="8">
         <f t="shared" si="0"/>
         <v>107.79400000000001</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E33" s="9">
         <v>538.97</v>
       </c>
-      <c r="G32" s="35">
+      <c r="G33" s="20">
         <f t="shared" si="1"/>
         <v>20.001286935281719</v>
       </c>
-      <c r="H32" s="35">
+      <c r="H33" s="20">
         <f t="shared" si="2"/>
         <v>-1.2869352817190816E-3</v>
       </c>
-      <c r="I32" s="35">
+      <c r="I33" s="20">
         <f t="shared" si="3"/>
         <v>-6.4346764085954078E-3</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="6">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="6">
         <v>30</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C34" s="9">
         <v>1116.73</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D34" s="8">
         <f t="shared" si="0"/>
         <v>111.673</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E34" s="9">
         <v>558.36</v>
       </c>
-      <c r="G33" s="35">
+      <c r="G34" s="20">
         <f t="shared" si="1"/>
         <v>30.000193615845649</v>
       </c>
-      <c r="H33" s="35">
+      <c r="H34" s="20">
         <f t="shared" si="2"/>
         <v>-1.936158456494752E-4</v>
       </c>
-      <c r="I33" s="35">
+      <c r="I34" s="20">
         <f t="shared" si="3"/>
         <v>-6.4538615216491735E-4</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="6">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="6">
         <v>40</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C35" s="9">
         <v>1155.4100000000001</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D35" s="8">
         <f t="shared" si="0"/>
         <v>115.54100000000001</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E35" s="9">
         <v>577.70000000000005</v>
       </c>
-      <c r="G34" s="35">
+      <c r="G35" s="20">
         <f t="shared" si="1"/>
         <v>40.000517853021371</v>
       </c>
-      <c r="H34" s="35">
+      <c r="H35" s="20">
         <f t="shared" si="2"/>
         <v>-5.1785302137119515E-4</v>
       </c>
-      <c r="I34" s="35">
+      <c r="I35" s="20">
         <f t="shared" si="3"/>
         <v>-1.2946325534279879E-3</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="6">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="6">
         <v>50</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C36" s="9">
         <v>1193.97</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D36" s="8">
         <f t="shared" si="0"/>
         <v>119.39700000000001</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E36" s="9">
         <v>596.99</v>
       </c>
-      <c r="G35" s="35">
+      <c r="G36" s="20">
         <f t="shared" si="1"/>
         <v>49.999675371066274</v>
       </c>
-      <c r="H35" s="35">
+      <c r="H36" s="20">
         <f t="shared" si="2"/>
         <v>3.2462893372553481E-4</v>
       </c>
-      <c r="I35" s="35">
+      <c r="I36" s="20">
         <f t="shared" si="3"/>
         <v>6.4925786745106961E-4</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="6">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
         <v>60</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C37" s="9">
         <v>1232.42</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D37" s="8">
         <f t="shared" si="0"/>
         <v>123.242</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E37" s="9">
         <v>616.21</v>
       </c>
-      <c r="G36" s="35">
+      <c r="G37" s="20">
         <f t="shared" si="1"/>
         <v>60.000260484511401</v>
       </c>
-      <c r="H36" s="35">
+      <c r="H37" s="20">
         <f t="shared" si="2"/>
         <v>-2.6048451140070483E-4</v>
       </c>
-      <c r="I36" s="35">
+      <c r="I37" s="20">
         <f t="shared" si="3"/>
         <v>-4.3414085233450805E-4</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="6">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="6">
         <v>70</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C38" s="9">
         <v>1270.75</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D38" s="8">
         <f t="shared" si="0"/>
         <v>127.075</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E38" s="9">
         <v>635.38</v>
       </c>
-      <c r="G37" s="35">
+      <c r="G38" s="20">
         <f t="shared" si="1"/>
         <v>69.999673411817639</v>
       </c>
-      <c r="H37" s="35">
+      <c r="H38" s="20">
         <f t="shared" si="2"/>
         <v>3.2658818236086518E-4</v>
       </c>
-      <c r="I37" s="35">
+      <c r="I38" s="20">
         <f t="shared" si="3"/>
         <v>4.6655454622980736E-4</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="6">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="6">
         <v>80</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C39" s="9">
         <v>1308.97</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D39" s="8">
         <f t="shared" si="0"/>
         <v>130.89699999999999</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E39" s="9">
         <v>654.48</v>
       </c>
-      <c r="G38" s="35">
+      <c r="G39" s="20">
         <f t="shared" si="1"/>
         <v>80.000524122790878</v>
       </c>
-      <c r="H38" s="35">
+      <c r="H39" s="20">
         <f t="shared" si="2"/>
         <v>-5.2412279087832303E-4</v>
       </c>
-      <c r="I38" s="35">
+      <c r="I39" s="20">
         <f t="shared" si="3"/>
         <v>-6.5515348859790379E-4</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="6">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="6">
         <v>90</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C40" s="9">
         <v>1347.07</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D40" s="8">
         <f t="shared" si="0"/>
         <v>134.70699999999999</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E40" s="9">
         <v>673.53</v>
       </c>
-      <c r="G39" s="35">
+      <c r="G40" s="20">
         <f t="shared" si="1"/>
         <v>90.000197142750253</v>
       </c>
-      <c r="H39" s="35">
+      <c r="H40" s="20">
         <f t="shared" si="2"/>
         <v>-1.9714275025251027E-4</v>
       </c>
-      <c r="I39" s="35">
+      <c r="I40" s="20">
         <f t="shared" si="3"/>
         <v>-2.1904750028056696E-4</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="6">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="6">
         <v>100</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C41" s="9">
         <v>1385.06</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D41" s="8">
         <f t="shared" si="0"/>
         <v>138.506</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E41" s="9">
         <v>692.53</v>
       </c>
-      <c r="G40" s="35">
+      <c r="G41" s="20">
         <f t="shared" si="1"/>
         <v>100.00131828754539</v>
       </c>
-      <c r="H40" s="35">
+      <c r="H41" s="20">
         <f t="shared" si="2"/>
         <v>-1.3182875453878751E-3</v>
       </c>
-      <c r="I40" s="35">
+      <c r="I41" s="20">
         <f t="shared" si="3"/>
         <v>-1.3182875453878751E-3</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="6">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="6">
         <v>110</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C42" s="9">
         <v>1422.93</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D42" s="8">
         <f t="shared" si="0"/>
         <v>142.29300000000001</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E42" s="9">
         <v>711.46</v>
       </c>
-      <c r="G41" s="35">
+      <c r="G42" s="20">
         <f t="shared" si="1"/>
         <v>110.00125619858775</v>
       </c>
-      <c r="H41" s="35">
+      <c r="H42" s="20">
         <f t="shared" si="2"/>
         <v>-1.2561985877539428E-3</v>
       </c>
-      <c r="I41" s="35">
+      <c r="I42" s="20">
         <f t="shared" si="3"/>
         <v>-1.1419987161399481E-3</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="6">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="6">
         <v>120</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C43" s="9">
         <v>1460.68</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D43" s="8">
         <f t="shared" si="0"/>
         <v>146.06800000000001</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E43" s="9">
         <v>730.34</v>
       </c>
-      <c r="G42" s="35">
+      <c r="G43" s="20">
         <f t="shared" si="1"/>
         <v>119.99999999999963</v>
       </c>
-      <c r="H42" s="35">
+      <c r="H43" s="20">
         <f t="shared" si="2"/>
         <v>3.694822225952521E-13</v>
       </c>
-      <c r="I42" s="35">
+      <c r="I43" s="20">
         <f t="shared" si="3"/>
         <v>3.079018521627101E-13</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="6">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="6">
         <v>130</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C44" s="9">
         <v>1498.32</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D44" s="8">
         <f t="shared" si="0"/>
         <v>149.83199999999999</v>
       </c>
-      <c r="E43" s="9">
+      <c r="E44" s="9">
         <v>749.16</v>
       </c>
-      <c r="G43" s="35">
+      <c r="G44" s="20">
         <f t="shared" si="1"/>
         <v>130.00019956628185</v>
       </c>
-      <c r="H43" s="35">
+      <c r="H44" s="20">
         <f t="shared" si="2"/>
         <v>-1.9956628185013869E-4</v>
       </c>
-      <c r="I43" s="35">
+      <c r="I44" s="20">
         <f t="shared" si="3"/>
         <v>-1.5351252450010669E-4</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="6">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="6">
         <v>140</v>
       </c>
-      <c r="C44" s="9">
+      <c r="C45" s="9">
         <v>1535.84</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D45" s="8">
         <f t="shared" si="0"/>
         <v>153.584</v>
       </c>
-      <c r="E44" s="9">
+      <c r="E45" s="9">
         <v>767.92</v>
       </c>
-      <c r="G44" s="35">
+      <c r="G45" s="20">
         <f t="shared" si="1"/>
         <v>139.99919927410693</v>
       </c>
-      <c r="H44" s="35">
+      <c r="H45" s="20">
         <f t="shared" si="2"/>
         <v>8.0072589307178532E-4</v>
       </c>
-      <c r="I44" s="35">
+      <c r="I45" s="20">
         <f t="shared" si="3"/>
         <v>5.7194706647984675E-4</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="6">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="6">
         <v>150</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C46" s="9">
         <v>1573.25</v>
       </c>
-      <c r="D45" s="8">
+      <c r="D46" s="8">
         <f t="shared" si="0"/>
         <v>157.32499999999999</v>
       </c>
-      <c r="E45" s="9">
+      <c r="E46" s="9">
         <v>786.63</v>
       </c>
-      <c r="G45" s="35">
+      <c r="G46" s="20">
         <f t="shared" si="1"/>
         <v>149.99966533247584</v>
       </c>
-      <c r="H45" s="35">
+      <c r="H46" s="20">
         <f t="shared" si="2"/>
         <v>3.3466752415733936E-4</v>
       </c>
-      <c r="I45" s="35">
+      <c r="I46" s="20">
         <f t="shared" si="3"/>
         <v>2.2311168277155957E-4</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="6">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="6">
         <v>160</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C47" s="9">
         <v>1610.54</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D47" s="8">
         <f t="shared" si="0"/>
         <v>161.054</v>
       </c>
-      <c r="E46" s="9">
+      <c r="E47" s="9">
         <v>805.27</v>
       </c>
-      <c r="G46" s="35">
+      <c r="G47" s="20">
         <f t="shared" si="1"/>
         <v>159.99892574208829</v>
       </c>
-      <c r="H46" s="35">
+      <c r="H47" s="20">
         <f t="shared" si="2"/>
         <v>1.0742579117106743E-3</v>
       </c>
-      <c r="I46" s="35">
+      <c r="I47" s="20">
         <f t="shared" si="3"/>
         <v>6.7141119481917144E-4</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="6">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="6">
         <v>170</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C48" s="9">
         <v>1647.72</v>
       </c>
-      <c r="D47" s="8">
+      <c r="D48" s="8">
         <f t="shared" si="0"/>
         <v>164.77199999999999</v>
       </c>
-      <c r="E47" s="9">
+      <c r="E48" s="9">
         <v>823.86</v>
       </c>
-      <c r="G47" s="35">
+      <c r="G48" s="20">
         <f t="shared" si="1"/>
         <v>169.99966324979189</v>
       </c>
-      <c r="H47" s="35">
+      <c r="H48" s="20">
         <f t="shared" si="2"/>
         <v>3.3675020810619571E-4</v>
       </c>
-      <c r="I47" s="35">
+      <c r="I48" s="20">
         <f t="shared" si="3"/>
         <v>1.9808835770952687E-4</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="6">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="6">
         <v>180</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C49" s="9">
         <v>1684.78</v>
       </c>
-      <c r="D48" s="8">
+      <c r="D49" s="8">
         <f t="shared" si="0"/>
         <v>168.47800000000001</v>
       </c>
-      <c r="E48" s="9">
+      <c r="E49" s="9">
         <v>842.39</v>
       </c>
-      <c r="G48" s="35">
+      <c r="G49" s="20">
         <f t="shared" si="1"/>
         <v>179.99918927693733</v>
       </c>
-      <c r="H48" s="35">
+      <c r="H49" s="20">
         <f t="shared" si="2"/>
         <v>8.1072306267060412E-4</v>
       </c>
-      <c r="I48" s="35">
+      <c r="I49" s="20">
         <f t="shared" si="3"/>
         <v>4.5040170148366896E-4</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="6">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="6">
         <v>190</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C50" s="9">
         <v>1721.73</v>
       </c>
-      <c r="D49" s="8">
+      <c r="D50" s="8">
         <f t="shared" si="0"/>
         <v>172.173</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E50" s="9">
         <v>860.86</v>
       </c>
-      <c r="G49" s="35">
+      <c r="G50" s="20">
         <f t="shared" si="1"/>
         <v>190.00020331540267</v>
       </c>
-      <c r="H49" s="35">
+      <c r="H50" s="20">
         <f t="shared" si="2"/>
         <v>-2.0331540267193304E-4</v>
       </c>
-      <c r="I49" s="35">
+      <c r="I50" s="20">
         <f t="shared" si="3"/>
         <v>-1.0700810666943844E-4</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="6">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="6">
         <v>200</v>
       </c>
-      <c r="C50" s="9">
+      <c r="C51" s="9">
         <v>1758.56</v>
       </c>
-      <c r="D50" s="8">
+      <c r="D51" s="8">
         <f t="shared" si="0"/>
         <v>175.85599999999999</v>
       </c>
-      <c r="E50" s="9">
+      <c r="E51" s="9">
         <v>879.28</v>
       </c>
-      <c r="G50" s="35">
+      <c r="G51" s="20">
         <f t="shared" si="1"/>
         <v>199.99999999999989</v>
       </c>
-      <c r="H50" s="35">
+      <c r="H51" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I50" s="35">
+      <c r="I51" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="6">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="6">
         <v>210</v>
       </c>
-      <c r="C51" s="9">
+      <c r="C52" s="9">
         <v>1795.28</v>
       </c>
-      <c r="D51" s="8">
+      <c r="D52" s="8">
         <f t="shared" si="0"/>
         <v>179.52799999999999</v>
       </c>
-      <c r="E51" s="9">
+      <c r="E52" s="9">
         <v>897.64</v>
       </c>
-      <c r="G51" s="35">
+      <c r="G52" s="20">
         <f t="shared" si="1"/>
         <v>210.00129577875438</v>
       </c>
-      <c r="H51" s="35">
+      <c r="H52" s="20">
         <f t="shared" si="2"/>
         <v>-1.2957787543825816E-3</v>
       </c>
-      <c r="I51" s="35">
+      <c r="I52" s="20">
         <f t="shared" si="3"/>
         <v>-6.170375020869436E-4</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="6">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="6">
         <v>220</v>
       </c>
-      <c r="C52" s="9">
+      <c r="C53" s="9">
         <v>1831.88</v>
       </c>
-      <c r="D52" s="8">
+      <c r="D53" s="8">
         <f t="shared" si="0"/>
         <v>183.18800000000002</v>
       </c>
-      <c r="E52" s="9">
+      <c r="E53" s="9">
         <v>915.94</v>
       </c>
-      <c r="G52" s="35">
+      <c r="G53" s="20">
         <f t="shared" si="1"/>
         <v>220.00136828884052</v>
       </c>
-      <c r="H52" s="35">
+      <c r="H53" s="20">
         <f t="shared" si="2"/>
         <v>-1.3682888405242011E-3</v>
       </c>
-      <c r="I52" s="35">
+      <c r="I53" s="20">
         <f t="shared" si="3"/>
         <v>-6.2194947296554596E-4</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="6">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="6">
         <v>230</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C54" s="9">
         <v>1868.36</v>
       </c>
-      <c r="D53" s="8">
+      <c r="D54" s="8">
         <f t="shared" si="0"/>
         <v>186.83599999999998</v>
       </c>
-      <c r="E53" s="9">
+      <c r="E54" s="9">
         <v>934.18</v>
       </c>
-      <c r="G53" s="35">
+      <c r="G54" s="20">
         <f t="shared" si="1"/>
         <v>230.00020589406736</v>
       </c>
-      <c r="H53" s="35">
+      <c r="H54" s="20">
         <f t="shared" si="2"/>
         <v>-2.0589406736348792E-4</v>
       </c>
-      <c r="I53" s="35">
+      <c r="I54" s="20">
         <f t="shared" si="3"/>
         <v>-8.9519159723255626E-5</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="6">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="6">
         <v>240</v>
       </c>
-      <c r="C54" s="9">
+      <c r="C55" s="9">
         <v>1904.73</v>
       </c>
-      <c r="D54" s="8">
+      <c r="D55" s="8">
         <f t="shared" si="0"/>
         <v>190.47300000000001</v>
       </c>
-      <c r="E54" s="9">
+      <c r="E55" s="9">
         <v>952.36</v>
       </c>
-      <c r="G54" s="35">
+      <c r="G55" s="20">
         <f t="shared" si="1"/>
         <v>240.00055079732715</v>
       </c>
-      <c r="H54" s="35">
+      <c r="H55" s="20">
         <f t="shared" si="2"/>
         <v>-5.5079732715057617E-4</v>
       </c>
-      <c r="I54" s="35">
+      <c r="I55" s="20">
         <f t="shared" si="3"/>
         <v>-2.2949888631274004E-4</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="6">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="6">
         <v>250</v>
       </c>
-      <c r="C55" s="9">
+      <c r="C56" s="9">
         <v>1940.98</v>
       </c>
-      <c r="D55" s="8">
+      <c r="D56" s="8">
         <f t="shared" si="0"/>
         <v>194.09800000000001</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E56" s="9">
         <v>970.49</v>
       </c>
-      <c r="G55" s="35">
+      <c r="G56" s="20">
         <f t="shared" si="1"/>
         <v>249.99965465322165</v>
       </c>
-      <c r="H55" s="35">
+      <c r="H56" s="20">
         <f t="shared" si="2"/>
         <v>3.4534677834585636E-4</v>
       </c>
-      <c r="I55" s="35">
+      <c r="I56" s="20">
         <f t="shared" si="3"/>
         <v>1.3813871133834256E-4</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="6">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="6">
         <v>260</v>
       </c>
-      <c r="C56" s="9">
+      <c r="C57" s="9">
         <v>1977.12</v>
       </c>
-      <c r="D56" s="8">
+      <c r="D57" s="8">
         <f t="shared" si="0"/>
         <v>197.71199999999999</v>
       </c>
-      <c r="E56" s="9">
+      <c r="E57" s="9">
         <v>988.56</v>
       </c>
-      <c r="G56" s="35">
+      <c r="G57" s="20">
         <f t="shared" si="1"/>
         <v>260.00027716187469</v>
       </c>
-      <c r="H56" s="35">
+      <c r="H57" s="20">
         <f t="shared" si="2"/>
         <v>-2.7716187469195575E-4</v>
       </c>
-      <c r="I56" s="35">
+      <c r="I57" s="20">
         <f t="shared" si="3"/>
         <v>-1.066007210353676E-4</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="6">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="6">
         <v>270</v>
       </c>
-      <c r="C57" s="9">
+      <c r="C58" s="9">
         <v>2013.14</v>
       </c>
-      <c r="D57" s="8">
+      <c r="D58" s="8">
         <f t="shared" si="0"/>
         <v>201.31400000000002</v>
       </c>
-      <c r="E57" s="9">
+      <c r="E58" s="9">
         <v>1006.57</v>
       </c>
-      <c r="G57" s="35">
+      <c r="G58" s="20">
         <f t="shared" si="1"/>
         <v>269.99965243505915</v>
       </c>
-      <c r="H57" s="35">
+      <c r="H58" s="20">
         <f t="shared" si="2"/>
         <v>3.4756494085286249E-4</v>
       </c>
-      <c r="I57" s="35">
+      <c r="I58" s="20">
         <f t="shared" si="3"/>
         <v>1.2872775587143055E-4</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="6">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="6">
         <v>280</v>
       </c>
-      <c r="C58" s="9">
+      <c r="C59" s="9">
         <v>2049.0500000000002</v>
       </c>
-      <c r="D58" s="8">
+      <c r="D59" s="8">
         <f t="shared" si="0"/>
         <v>204.90500000000003</v>
       </c>
-      <c r="E58" s="9">
+      <c r="E59" s="9">
         <v>1024.52</v>
       </c>
-      <c r="G58" s="35">
+      <c r="G59" s="20">
         <f t="shared" si="1"/>
         <v>280.00055789566778</v>
       </c>
-      <c r="H58" s="35">
+      <c r="H59" s="20">
         <f t="shared" si="2"/>
         <v>-5.5789566778230437E-4</v>
       </c>
-      <c r="I58" s="35">
+      <c r="I59" s="20">
         <f t="shared" si="3"/>
         <v>-1.9924845277939442E-4</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="6">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="6">
         <v>290</v>
       </c>
-      <c r="C59" s="9">
+      <c r="C60" s="9">
         <v>2084.84</v>
       </c>
-      <c r="D59" s="8">
+      <c r="D60" s="8">
         <f t="shared" si="0"/>
         <v>208.48400000000001</v>
       </c>
-      <c r="E59" s="9">
+      <c r="E60" s="9">
         <v>1042.42</v>
       </c>
-      <c r="G59" s="35">
+      <c r="G60" s="20">
         <f t="shared" si="1"/>
         <v>290.00020988708764</v>
       </c>
-      <c r="H59" s="35">
+      <c r="H60" s="20">
         <f t="shared" si="2"/>
         <v>-2.098870876352521E-4</v>
       </c>
-      <c r="I59" s="35">
+      <c r="I60" s="20">
         <f t="shared" si="3"/>
         <v>-7.2374857805259342E-5</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="6">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="6">
         <v>300</v>
       </c>
-      <c r="C60" s="9">
+      <c r="C61" s="9">
         <v>2120.52</v>
       </c>
-      <c r="D60" s="8">
+      <c r="D61" s="8">
         <f t="shared" si="0"/>
         <v>212.05199999999999</v>
       </c>
-      <c r="E60" s="9">
+      <c r="E61" s="9">
         <v>1060.26</v>
       </c>
-      <c r="G60" s="35">
+      <c r="G61" s="20">
         <f t="shared" si="1"/>
         <v>300.00140378492262</v>
       </c>
-      <c r="H60" s="35">
+      <c r="H61" s="20">
         <f t="shared" si="2"/>
         <v>-1.4037849226156141E-3</v>
       </c>
-      <c r="I60" s="35">
+      <c r="I61" s="20">
         <f t="shared" si="3"/>
         <v>-4.6792830753853803E-4</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="6">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="6">
         <v>310</v>
       </c>
-      <c r="C61" s="9">
+      <c r="C62" s="9">
         <v>2156.08</v>
       </c>
-      <c r="D61" s="8">
+      <c r="D62" s="8">
         <f t="shared" si="0"/>
         <v>215.608</v>
       </c>
-      <c r="E61" s="9">
+      <c r="E62" s="9">
         <v>1078.04</v>
       </c>
-      <c r="G61" s="35">
+      <c r="G62" s="20">
         <f t="shared" si="1"/>
         <v>310.0013379342393</v>
       </c>
-      <c r="H61" s="35">
+      <c r="H62" s="20">
         <f t="shared" si="2"/>
         <v>-1.3379342393022853E-3</v>
       </c>
-      <c r="I61" s="35">
+      <c r="I62" s="20">
         <f t="shared" si="3"/>
         <v>-4.3159169009751141E-4</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="6">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="6">
         <v>320</v>
       </c>
-      <c r="C62" s="9">
+      <c r="C63" s="9">
         <v>2191.52</v>
       </c>
-      <c r="D62" s="8">
+      <c r="D63" s="8">
         <f t="shared" si="0"/>
         <v>219.15199999999999</v>
       </c>
-      <c r="E62" s="9">
+      <c r="E63" s="9">
         <v>1095.76</v>
       </c>
-      <c r="G62" s="35">
+      <c r="G63" s="20">
         <f t="shared" si="1"/>
         <v>319.99999999999989</v>
       </c>
-      <c r="H62" s="35">
+      <c r="H63" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I62" s="35">
+      <c r="I63" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="6">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="6">
         <v>330</v>
       </c>
-      <c r="C63" s="9">
+      <c r="C64" s="9">
         <v>2226.85</v>
       </c>
-      <c r="D63" s="8">
+      <c r="D64" s="8">
         <f t="shared" si="0"/>
         <v>222.685</v>
       </c>
-      <c r="E63" s="9">
+      <c r="E64" s="9">
         <v>1113.42</v>
       </c>
-      <c r="G63" s="35">
+      <c r="G64" s="20">
         <f t="shared" si="1"/>
         <v>330.00021263627156</v>
       </c>
-      <c r="H63" s="35">
+      <c r="H64" s="20">
         <f t="shared" si="2"/>
         <v>-2.1263627155576614E-4</v>
       </c>
-      <c r="I63" s="35">
+      <c r="I64" s="20">
         <f t="shared" si="3"/>
         <v>-6.4435233804777624E-5</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="6">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="6">
         <v>340</v>
       </c>
-      <c r="C64" s="9">
+      <c r="C65" s="9">
         <v>2262.06</v>
       </c>
-      <c r="D64" s="8">
+      <c r="D65" s="8">
         <f t="shared" si="0"/>
         <v>226.20599999999999</v>
       </c>
-      <c r="E64" s="9">
+      <c r="E65" s="9">
         <v>1131.03</v>
       </c>
-      <c r="G64" s="35">
+      <c r="G65" s="20">
         <f t="shared" si="1"/>
         <v>339.99914666071805</v>
       </c>
-      <c r="H64" s="35">
+      <c r="H65" s="20">
         <f t="shared" si="2"/>
         <v>8.5333928194586406E-4</v>
       </c>
-      <c r="I64" s="35">
+      <c r="I65" s="20">
         <f t="shared" si="3"/>
         <v>2.5098214174878357E-4</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B65" s="6">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="6">
         <v>350</v>
       </c>
-      <c r="C65" s="9">
+      <c r="C66" s="9">
         <v>2297.16</v>
       </c>
-      <c r="D65" s="8">
+      <c r="D66" s="8">
         <f t="shared" si="0"/>
         <v>229.71599999999998</v>
       </c>
-      <c r="E65" s="9">
+      <c r="E66" s="9">
         <v>1148.58</v>
       </c>
-      <c r="G65" s="35">
+      <c r="G66" s="20">
         <f t="shared" si="1"/>
         <v>349.99964326995132</v>
       </c>
-      <c r="H65" s="35">
+      <c r="H66" s="20">
         <f t="shared" si="2"/>
         <v>3.5673004867931013E-4</v>
       </c>
-      <c r="I65" s="35">
+      <c r="I66" s="20">
         <f t="shared" si="3"/>
         <v>1.0192287105123146E-4</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B66" s="6">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="6">
         <v>360</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C67" s="9">
         <v>2332.14</v>
       </c>
-      <c r="D66" s="8">
+      <c r="D67" s="8">
         <f t="shared" si="0"/>
         <v>233.214</v>
       </c>
-      <c r="E66" s="9">
+      <c r="E67" s="9">
         <v>1166.07</v>
       </c>
-      <c r="G66" s="35">
+      <c r="G67" s="20">
         <f t="shared" si="1"/>
         <v>359.99885468883519</v>
       </c>
-      <c r="H66" s="35">
+      <c r="H67" s="20">
         <f t="shared" si="2"/>
         <v>1.1453111648052072E-3</v>
       </c>
-      <c r="I66" s="35">
+      <c r="I67" s="20">
         <f t="shared" si="3"/>
         <v>3.1814199022366866E-4</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" s="6">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="6">
         <v>370</v>
       </c>
-      <c r="C67" s="9">
+      <c r="C68" s="9">
         <v>2367.0100000000002</v>
       </c>
-      <c r="D67" s="8">
+      <c r="D68" s="8">
         <f t="shared" si="0"/>
         <v>236.70100000000002</v>
       </c>
-      <c r="E67" s="9">
+      <c r="E68" s="9">
         <v>1183.51</v>
       </c>
-      <c r="G67" s="35">
+      <c r="G68" s="20">
         <f t="shared" si="1"/>
         <v>369.99964090264842</v>
       </c>
-      <c r="H67" s="35">
+      <c r="H68" s="20">
         <f t="shared" si="2"/>
         <v>3.5909735157702016E-4</v>
       </c>
-      <c r="I67" s="35">
+      <c r="I68" s="20">
         <f t="shared" si="3"/>
         <v>9.7053338264059498E-5</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B68" s="6">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="6">
         <v>380</v>
       </c>
-      <c r="C68" s="9">
+      <c r="C69" s="9">
         <v>2401.7600000000002</v>
       </c>
-      <c r="D68" s="8">
+      <c r="D69" s="8">
         <f t="shared" si="0"/>
         <v>240.17600000000002</v>
       </c>
-      <c r="E68" s="9">
+      <c r="E69" s="9">
         <v>1200.8800000000001</v>
       </c>
-      <c r="G68" s="35">
+      <c r="G69" s="20">
         <f t="shared" si="1"/>
         <v>379.99913529729378</v>
       </c>
-      <c r="H68" s="35">
+      <c r="H69" s="20">
         <f t="shared" si="2"/>
         <v>8.6470270622385215E-4</v>
       </c>
-      <c r="I68" s="35">
+      <c r="I69" s="20">
         <f t="shared" si="3"/>
         <v>2.2755334374311898E-4</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" s="6">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" s="6">
         <v>390</v>
       </c>
-      <c r="C69" s="9">
+      <c r="C70" s="9">
         <v>2436.4</v>
       </c>
-      <c r="D69" s="8">
+      <c r="D70" s="8">
         <f t="shared" si="0"/>
         <v>243.64000000000001</v>
       </c>
-      <c r="E69" s="9">
+      <c r="E70" s="9">
         <v>1218.2</v>
       </c>
-      <c r="G69" s="35">
+      <c r="G70" s="20">
         <f t="shared" si="1"/>
         <v>390.00021689779101</v>
       </c>
-      <c r="H69" s="35">
+      <c r="H70" s="20">
         <f t="shared" si="2"/>
         <v>-2.1689779100597661E-4</v>
       </c>
-      <c r="I69" s="35">
+      <c r="I70" s="20">
         <f t="shared" si="3"/>
         <v>-5.5614818206660668E-5</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B70" s="6">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" s="6">
         <v>400</v>
       </c>
-      <c r="C70" s="9">
+      <c r="C71" s="9">
         <v>2470.92</v>
       </c>
-      <c r="D70" s="8">
+      <c r="D71" s="8">
         <f t="shared" si="0"/>
         <v>247.09200000000001</v>
       </c>
-      <c r="E70" s="9">
+      <c r="E71" s="9">
         <v>1235.46</v>
       </c>
-      <c r="G70" s="35">
+      <c r="G71" s="20">
         <f t="shared" si="1"/>
         <v>399.99999999999977</v>
       </c>
-      <c r="H70" s="35">
+      <c r="H71" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I70" s="35">
+      <c r="I71" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B71" s="6">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="6">
         <v>410</v>
       </c>
-      <c r="C71" s="9">
+      <c r="C72" s="9">
         <v>2505.33</v>
       </c>
-      <c r="D71" s="8">
+      <c r="D72" s="8">
         <f t="shared" si="0"/>
         <v>250.53299999999999</v>
       </c>
-      <c r="E71" s="9">
+      <c r="E72" s="9">
         <v>1252.6600000000001</v>
       </c>
-      <c r="G71" s="35">
+      <c r="G72" s="20">
         <f t="shared" si="1"/>
         <v>410.00138292484286</v>
       </c>
-      <c r="H71" s="35">
+      <c r="H72" s="20">
         <f t="shared" si="2"/>
         <v>-1.3829248428578467E-3</v>
       </c>
-      <c r="I71" s="35">
+      <c r="I72" s="20">
         <f t="shared" si="3"/>
         <v>-3.3729874216045043E-4</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B72" s="6">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="6">
         <v>420</v>
       </c>
-      <c r="C72" s="9">
+      <c r="C73" s="9">
         <v>2539.62</v>
       </c>
-      <c r="D72" s="8">
+      <c r="D73" s="8">
         <f t="shared" si="0"/>
         <v>253.96199999999999</v>
       </c>
-      <c r="E72" s="9">
+      <c r="E73" s="9">
         <v>1269.81</v>
       </c>
-      <c r="G72" s="35">
+      <c r="G73" s="20">
         <f t="shared" si="1"/>
         <v>420.00146062200002</v>
       </c>
-      <c r="H72" s="35">
+      <c r="H73" s="20">
         <f t="shared" si="2"/>
         <v>-1.460622000024614E-3</v>
       </c>
-      <c r="I72" s="35">
+      <c r="I73" s="20">
         <f t="shared" si="3"/>
         <v>-3.4776714286300329E-4</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" s="6">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B74" s="6">
         <v>430</v>
       </c>
-      <c r="C73" s="9">
+      <c r="C74" s="9">
         <v>2573.79</v>
       </c>
-      <c r="D73" s="8">
+      <c r="D74" s="8">
         <f t="shared" si="0"/>
         <v>257.37900000000002</v>
       </c>
-      <c r="E73" s="9">
+      <c r="E74" s="9">
         <v>1286.8900000000001</v>
       </c>
-      <c r="G73" s="35">
+      <c r="G74" s="20">
         <f t="shared" si="1"/>
         <v>430.0002198349851</v>
       </c>
-      <c r="H73" s="35">
+      <c r="H74" s="20">
         <f t="shared" si="2"/>
         <v>-2.1983498510280697E-4</v>
       </c>
-      <c r="I73" s="35">
+      <c r="I74" s="20">
         <f t="shared" si="3"/>
         <v>-5.1124415140187662E-5</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B74" s="6">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="6">
         <v>440</v>
       </c>
-      <c r="C74" s="9">
+      <c r="C75" s="9">
         <v>2607.85</v>
       </c>
-      <c r="D74" s="8">
+      <c r="D75" s="8">
         <f t="shared" si="0"/>
         <v>260.78499999999997</v>
       </c>
-      <c r="E74" s="9">
+      <c r="E75" s="9">
         <v>1303.92</v>
       </c>
-      <c r="G74" s="35">
+      <c r="G75" s="20">
         <f t="shared" si="1"/>
         <v>440.00058821805231</v>
       </c>
-      <c r="H74" s="35">
+      <c r="H75" s="20">
         <f t="shared" si="2"/>
         <v>-5.8821805231445978E-4</v>
       </c>
-      <c r="I74" s="35">
+      <c r="I75" s="20">
         <f t="shared" si="3"/>
         <v>-1.3368592098055905E-4</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B75" s="6">
-        <v>450</v>
-      </c>
-      <c r="C75" s="9">
-        <v>2641.79</v>
-      </c>
-      <c r="D75" s="8">
-        <f t="shared" ref="D75:D115" si="4">C75/10</f>
-        <v>264.17899999999997</v>
-      </c>
-      <c r="E75" s="9">
-        <v>1320.9</v>
-      </c>
-      <c r="G75" s="35">
-        <f t="shared" ref="G75:G115" si="5">(-$C$5+SQRT($C$5*$C$5-4*$C$6*(1-C75/1000)))/(2*$C$6)</f>
-        <v>449.99963111067495</v>
-      </c>
-      <c r="H75" s="35">
-        <f t="shared" ref="H75:H115" si="6">B75-G75</f>
-        <v>3.688893250455294E-4</v>
-      </c>
-      <c r="I75" s="35">
-        <f t="shared" ref="I75:I115" si="7">H75/B75*100</f>
-        <v>8.1975405565673208E-5</v>
-      </c>
-    </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="6">
+        <v>450</v>
+      </c>
+      <c r="C76" s="9">
+        <v>2641.79</v>
+      </c>
+      <c r="D76" s="8">
+        <f t="shared" ref="D76:D116" si="4">C76/10</f>
+        <v>264.17899999999997</v>
+      </c>
+      <c r="E76" s="9">
+        <v>1320.9</v>
+      </c>
+      <c r="G76" s="20">
+        <f t="shared" ref="G76:G116" si="5">(-$C$6+SQRT($C$6*$C$6-4*$C$7*(1-C76/1000)))/(2*$C$7)</f>
+        <v>449.99963111067495</v>
+      </c>
+      <c r="H76" s="20">
+        <f t="shared" ref="H76:H116" si="6">B76-G76</f>
+        <v>3.688893250455294E-4</v>
+      </c>
+      <c r="I76" s="20">
+        <f t="shared" ref="I76:I116" si="7">H76/B76*100</f>
+        <v>8.1975405565673208E-5</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="6">
         <v>460</v>
       </c>
-      <c r="C76" s="9">
+      <c r="C77" s="9">
         <v>2675.62</v>
       </c>
-      <c r="D76" s="8">
+      <c r="D77" s="8">
         <f t="shared" si="4"/>
         <v>267.56200000000001</v>
       </c>
-      <c r="E76" s="9">
+      <c r="E77" s="9">
         <v>1337.81</v>
       </c>
-      <c r="G76" s="35">
+      <c r="G77" s="20">
         <f t="shared" si="5"/>
         <v>460.00029612083227</v>
       </c>
-      <c r="H76" s="35">
+      <c r="H77" s="20">
         <f t="shared" si="6"/>
         <v>-2.9612083227448238E-4</v>
       </c>
-      <c r="I76" s="35">
+      <c r="I77" s="20">
         <f t="shared" si="7"/>
         <v>-6.4374093972713553E-5</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B77" s="6">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B78" s="6">
         <v>470</v>
       </c>
-      <c r="C77" s="9">
+      <c r="C78" s="9">
         <v>2709.33</v>
       </c>
-      <c r="D77" s="8">
+      <c r="D78" s="8">
         <f t="shared" si="4"/>
         <v>270.93299999999999</v>
       </c>
-      <c r="E77" s="9">
+      <c r="E78" s="9">
         <v>1354.67</v>
       </c>
-      <c r="G77" s="35">
+      <c r="G78" s="20">
         <f t="shared" si="5"/>
         <v>469.99962857866831</v>
       </c>
-      <c r="H77" s="35">
+      <c r="H78" s="20">
         <f t="shared" si="6"/>
         <v>3.7142133169254521E-4</v>
       </c>
-      <c r="I77" s="35">
+      <c r="I78" s="20">
         <f t="shared" si="7"/>
         <v>7.9025815253733021E-5</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" s="6">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B79" s="6">
         <v>480</v>
       </c>
-      <c r="C78" s="9">
+      <c r="C79" s="9">
         <v>2742.93</v>
       </c>
-      <c r="D78" s="8">
+      <c r="D79" s="8">
         <f t="shared" si="4"/>
         <v>274.29300000000001</v>
       </c>
-      <c r="E78" s="9">
+      <c r="E79" s="9">
         <v>1371.46</v>
       </c>
-      <c r="G78" s="35">
+      <c r="G79" s="20">
         <f t="shared" si="5"/>
         <v>480.00059632076216</v>
       </c>
-      <c r="H78" s="35">
+      <c r="H79" s="20">
         <f t="shared" si="6"/>
         <v>-5.9632076215621055E-4</v>
       </c>
-      <c r="I78" s="35">
+      <c r="I79" s="20">
         <f t="shared" si="7"/>
         <v>-1.242334921158772E-4</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B79" s="6">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="6">
         <v>490</v>
       </c>
-      <c r="C79" s="9">
+      <c r="C80" s="9">
         <v>2776.41</v>
       </c>
-      <c r="D79" s="8">
+      <c r="D80" s="8">
         <f t="shared" si="4"/>
         <v>277.64099999999996</v>
       </c>
-      <c r="E79" s="9">
+      <c r="E80" s="9">
         <v>1388.2</v>
       </c>
-      <c r="G79" s="35">
+      <c r="G80" s="20">
         <f t="shared" si="5"/>
         <v>490.00022439302546</v>
       </c>
-      <c r="H79" s="35">
+      <c r="H80" s="20">
         <f t="shared" si="6"/>
         <v>-2.2439302546217732E-4</v>
       </c>
-      <c r="I79" s="35">
+      <c r="I80" s="20">
         <f t="shared" si="7"/>
         <v>-4.579449499228108E-5</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B80" s="6">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="6">
         <v>500</v>
       </c>
-      <c r="C80" s="9">
+      <c r="C81" s="9">
         <v>2809.78</v>
       </c>
-      <c r="D80" s="8">
+      <c r="D81" s="8">
         <f t="shared" si="4"/>
         <v>280.97800000000001</v>
       </c>
-      <c r="E80" s="9">
+      <c r="E81" s="9">
         <v>1404.89</v>
       </c>
-      <c r="G80" s="35">
+      <c r="G81" s="20">
         <f t="shared" si="5"/>
         <v>500.00150114125745</v>
       </c>
-      <c r="H80" s="35">
+      <c r="H81" s="20">
         <f t="shared" si="6"/>
         <v>-1.5011412574494898E-3</v>
       </c>
-      <c r="I80" s="35">
+      <c r="I81" s="20">
         <f t="shared" si="7"/>
         <v>-3.0022825148989796E-4</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="6">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="6">
         <v>510</v>
       </c>
-      <c r="C81" s="9">
+      <c r="C82" s="9">
         <v>2843.03</v>
       </c>
-      <c r="D81" s="8">
+      <c r="D82" s="8">
         <f t="shared" si="4"/>
         <v>284.303</v>
       </c>
-      <c r="E81" s="9">
+      <c r="E82" s="9">
         <v>1421.51</v>
       </c>
-      <c r="G81" s="35">
+      <c r="G82" s="20">
         <f t="shared" si="5"/>
         <v>510.00143104652619</v>
       </c>
-      <c r="H81" s="35">
+      <c r="H82" s="20">
         <f t="shared" si="6"/>
         <v>-1.4310465261928584E-3</v>
       </c>
-      <c r="I81" s="35">
+      <c r="I82" s="20">
         <f t="shared" si="7"/>
         <v>-2.8059735807703108E-4</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B82" s="6">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="6">
         <v>520</v>
       </c>
-      <c r="C82" s="9">
+      <c r="C83" s="9">
         <v>2876.16</v>
       </c>
-      <c r="D82" s="8">
+      <c r="D83" s="8">
         <f t="shared" si="4"/>
         <v>287.61599999999999</v>
       </c>
-      <c r="E82" s="9">
+      <c r="E83" s="9">
         <v>1438.08</v>
       </c>
-      <c r="G82" s="35">
+      <c r="G83" s="20">
         <f t="shared" si="5"/>
         <v>519.99999999999977</v>
       </c>
-      <c r="H82" s="35">
+      <c r="H83" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I82" s="35">
+      <c r="I83" s="20">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="6">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="6">
         <v>530</v>
       </c>
-      <c r="C83" s="9">
+      <c r="C84" s="9">
         <v>2909.18</v>
       </c>
-      <c r="D83" s="8">
+      <c r="D84" s="8">
         <f t="shared" si="4"/>
         <v>290.91800000000001</v>
       </c>
-      <c r="E83" s="9">
+      <c r="E84" s="9">
         <v>1454.59</v>
       </c>
-      <c r="G83" s="35">
+      <c r="G84" s="20">
         <f t="shared" si="5"/>
         <v>530.00022753819724</v>
       </c>
-      <c r="H83" s="35">
+      <c r="H84" s="20">
         <f t="shared" si="6"/>
         <v>-2.2753819723675406E-4</v>
       </c>
-      <c r="I83" s="35">
+      <c r="I84" s="20">
         <f t="shared" si="7"/>
         <v>-4.2931735327689444E-5</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B84" s="6">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="6">
         <v>540</v>
       </c>
-      <c r="C84" s="9">
+      <c r="C85" s="9">
         <v>2942.08</v>
       </c>
-      <c r="D84" s="8">
+      <c r="D85" s="8">
         <f t="shared" si="4"/>
         <v>294.20799999999997</v>
       </c>
-      <c r="E84" s="9">
+      <c r="E85" s="9">
         <v>1471.04</v>
       </c>
-      <c r="G84" s="35">
+      <c r="G85" s="20">
         <f t="shared" si="5"/>
         <v>539.99908664692225</v>
       </c>
-      <c r="H84" s="35">
+      <c r="H85" s="20">
         <f t="shared" si="6"/>
         <v>9.1335307774897956E-4</v>
       </c>
-      <c r="I84" s="35">
+      <c r="I85" s="20">
         <f t="shared" si="7"/>
         <v>1.6913945884240361E-4</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B85" s="6">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="6">
         <v>550</v>
       </c>
-      <c r="C85" s="9">
+      <c r="C86" s="9">
         <v>2974.87</v>
       </c>
-      <c r="D85" s="8">
+      <c r="D86" s="8">
         <f t="shared" si="4"/>
         <v>297.48699999999997</v>
       </c>
-      <c r="E85" s="9">
+      <c r="E86" s="9">
         <v>1487.44</v>
       </c>
-      <c r="G85" s="35">
+      <c r="G86" s="20">
         <f t="shared" si="5"/>
         <v>549.99961809324145</v>
       </c>
-      <c r="H85" s="35">
+      <c r="H86" s="20">
         <f t="shared" si="6"/>
         <v>3.8190675854821166E-4</v>
       </c>
-      <c r="I85" s="35">
+      <c r="I86" s="20">
         <f t="shared" si="7"/>
         <v>6.9437592463311205E-5</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B86" s="6">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="6">
         <v>560</v>
       </c>
-      <c r="C86" s="9">
+      <c r="C87" s="9">
         <v>3007.54</v>
       </c>
-      <c r="D86" s="8">
+      <c r="D87" s="8">
         <f t="shared" si="4"/>
         <v>300.75400000000002</v>
       </c>
-      <c r="E86" s="9">
+      <c r="E87" s="9">
         <v>1503.77</v>
       </c>
-      <c r="G86" s="35">
+      <c r="G87" s="20">
         <f t="shared" si="5"/>
         <v>559.99877357070932</v>
       </c>
-      <c r="H86" s="35">
+      <c r="H87" s="20">
         <f t="shared" si="6"/>
         <v>1.2264292906820629E-3</v>
       </c>
-      <c r="I86" s="35">
+      <c r="I87" s="20">
         <f t="shared" si="7"/>
         <v>2.1900523047893982E-4</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B87" s="6">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B88" s="6">
         <v>570</v>
       </c>
-      <c r="C87" s="9">
+      <c r="C88" s="9">
         <v>3040.1</v>
       </c>
-      <c r="D87" s="8">
+      <c r="D88" s="8">
         <f t="shared" si="4"/>
         <v>304.01</v>
       </c>
-      <c r="E87" s="9">
+      <c r="E88" s="9">
         <v>1520.05</v>
       </c>
-      <c r="G87" s="35">
+      <c r="G88" s="20">
         <f t="shared" si="5"/>
         <v>569.99961537872423</v>
       </c>
-      <c r="H87" s="35">
+      <c r="H88" s="20">
         <f t="shared" si="6"/>
         <v>3.8462127577076899E-4</v>
       </c>
-      <c r="I87" s="35">
+      <c r="I88" s="20">
         <f t="shared" si="7"/>
         <v>6.7477416801889299E-5</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B88" s="6">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B89" s="6">
         <v>580</v>
       </c>
-      <c r="C88" s="9">
+      <c r="C89" s="9">
         <v>3072.54</v>
       </c>
-      <c r="D88" s="8">
+      <c r="D89" s="8">
         <f t="shared" si="4"/>
         <v>307.25400000000002</v>
       </c>
-      <c r="E88" s="9">
+      <c r="E89" s="9">
         <v>1536.27</v>
       </c>
-      <c r="G88" s="35">
+      <c r="G89" s="20">
         <f t="shared" si="5"/>
         <v>579.99907361675378</v>
       </c>
-      <c r="H88" s="35">
+      <c r="H89" s="20">
         <f t="shared" si="6"/>
         <v>9.2638324622384971E-4</v>
       </c>
-      <c r="I88" s="35">
+      <c r="I89" s="20">
         <f t="shared" si="7"/>
         <v>1.5972124934893959E-4</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B89" s="6">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="6">
         <v>590</v>
       </c>
-      <c r="C89" s="9">
+      <c r="C90" s="9">
         <v>3104.87</v>
       </c>
-      <c r="D89" s="8">
+      <c r="D90" s="8">
         <f t="shared" si="4"/>
         <v>310.48699999999997</v>
       </c>
-      <c r="E89" s="9">
+      <c r="E90" s="9">
         <v>1552.43</v>
       </c>
-      <c r="G89" s="35">
+      <c r="G90" s="20">
         <f t="shared" si="5"/>
         <v>590.00023242482007</v>
       </c>
-      <c r="H89" s="35">
+      <c r="H90" s="20">
         <f t="shared" si="6"/>
         <v>-2.3242482006935461E-4</v>
       </c>
-      <c r="I89" s="35">
+      <c r="I90" s="20">
         <f t="shared" si="7"/>
         <v>-3.9394037299890616E-5</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B90" s="6">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="6">
         <v>600</v>
       </c>
-      <c r="C90" s="9">
+      <c r="C91" s="9">
         <v>3137.08</v>
       </c>
-      <c r="D90" s="8">
+      <c r="D91" s="8">
         <f t="shared" si="4"/>
         <v>313.70799999999997</v>
       </c>
-      <c r="E90" s="9">
+      <c r="E91" s="9">
         <v>1568.54</v>
       </c>
-      <c r="G90" s="35">
+      <c r="G91" s="20">
         <f t="shared" si="5"/>
         <v>599.99999999999966</v>
       </c>
-      <c r="H90" s="35">
+      <c r="H91" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I90" s="35">
+      <c r="I91" s="20">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B91" s="6">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="6">
         <v>610</v>
       </c>
-      <c r="C91" s="9">
+      <c r="C92" s="9">
         <v>3169.18</v>
       </c>
-      <c r="D91" s="8">
+      <c r="D92" s="8">
         <f t="shared" si="4"/>
         <v>316.91800000000001</v>
       </c>
-      <c r="E91" s="9">
+      <c r="E92" s="9">
         <v>1584.59</v>
       </c>
-      <c r="G91" s="35">
+      <c r="G92" s="20">
         <f t="shared" si="5"/>
         <v>610.00148263793017</v>
       </c>
-      <c r="H91" s="35">
+      <c r="H92" s="20">
         <f t="shared" si="6"/>
         <v>-1.4826379301666748E-3</v>
       </c>
-      <c r="I91" s="35">
+      <c r="I92" s="20">
         <f t="shared" si="7"/>
         <v>-2.4305539838797945E-4</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B92" s="6">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="6">
         <v>620</v>
       </c>
-      <c r="C92" s="9">
+      <c r="C93" s="9">
         <v>3201.16</v>
       </c>
-      <c r="D92" s="8">
+      <c r="D93" s="8">
         <f t="shared" si="4"/>
         <v>320.11599999999999</v>
       </c>
-      <c r="E92" s="9">
+      <c r="E93" s="9">
         <v>1600.58</v>
       </c>
-      <c r="G92" s="35">
+      <c r="G93" s="20">
         <f t="shared" si="5"/>
         <v>620.00156631834341</v>
       </c>
-      <c r="H92" s="35">
+      <c r="H93" s="20">
         <f t="shared" si="6"/>
         <v>-1.566318343407147E-3</v>
       </c>
-      <c r="I92" s="35">
+      <c r="I93" s="20">
         <f t="shared" si="7"/>
         <v>-2.5263199087212048E-4</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B93" s="6">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="6">
         <v>630</v>
       </c>
-      <c r="C93" s="9">
+      <c r="C94" s="9">
         <v>3233.02</v>
       </c>
-      <c r="D93" s="8">
+      <c r="D94" s="8">
         <f t="shared" si="4"/>
         <v>323.30200000000002</v>
       </c>
-      <c r="E93" s="9">
+      <c r="E94" s="9">
         <v>1616.51</v>
       </c>
-      <c r="G93" s="35">
+      <c r="G94" s="20">
         <f t="shared" si="5"/>
         <v>630.00023580086804</v>
       </c>
-      <c r="H93" s="35">
+      <c r="H94" s="20">
         <f t="shared" si="6"/>
         <v>-2.3580086804031453E-4</v>
       </c>
-      <c r="I93" s="35">
+      <c r="I94" s="20">
         <f t="shared" si="7"/>
         <v>-3.7428709212748338E-5</v>
       </c>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B94" s="6">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="6">
         <v>640</v>
       </c>
-      <c r="C94" s="9">
+      <c r="C95" s="9">
         <v>3264.77</v>
       </c>
-      <c r="D94" s="8">
+      <c r="D95" s="8">
         <f t="shared" si="4"/>
         <v>326.47699999999998</v>
       </c>
-      <c r="E94" s="9">
+      <c r="E95" s="9">
         <v>1632.38</v>
       </c>
-      <c r="G94" s="35">
+      <c r="G95" s="20">
         <f t="shared" si="5"/>
         <v>640.00063109407392</v>
       </c>
-      <c r="H94" s="35">
+      <c r="H95" s="20">
         <f t="shared" si="6"/>
         <v>-6.3109407392403227E-4</v>
       </c>
-      <c r="I94" s="35">
+      <c r="I95" s="20">
         <f t="shared" si="7"/>
         <v>-9.8608449050630043E-5</v>
       </c>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B95" s="6">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="6">
         <v>650</v>
       </c>
-      <c r="C95" s="9">
+      <c r="C96" s="9">
         <v>3296.4</v>
       </c>
-      <c r="D95" s="8">
+      <c r="D96" s="8">
         <f t="shared" si="4"/>
         <v>329.64</v>
       </c>
-      <c r="E95" s="9">
+      <c r="E96" s="9">
         <v>1648.2</v>
       </c>
-      <c r="G95" s="35">
+      <c r="G96" s="20">
         <f t="shared" si="5"/>
         <v>649.99960412347843</v>
       </c>
-      <c r="H95" s="35">
+      <c r="H96" s="20">
         <f t="shared" si="6"/>
         <v>3.9587652156569675E-4</v>
       </c>
-      <c r="I95" s="35">
+      <c r="I96" s="20">
         <f t="shared" si="7"/>
         <v>6.0904080240876421E-5</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B96" s="6">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B97" s="6">
         <v>660</v>
       </c>
-      <c r="C96" s="9">
+      <c r="C97" s="9">
         <v>3327.92</v>
       </c>
-      <c r="D96" s="8">
+      <c r="D97" s="8">
         <f t="shared" si="4"/>
         <v>332.79200000000003</v>
       </c>
-      <c r="E96" s="9">
+      <c r="E97" s="9">
         <v>1663.96</v>
       </c>
-      <c r="G96" s="35">
+      <c r="G97" s="20">
         <f t="shared" si="5"/>
         <v>660.00031786397267</v>
       </c>
-      <c r="H96" s="35">
+      <c r="H97" s="20">
         <f t="shared" si="6"/>
         <v>-3.1786397266841959E-4</v>
       </c>
-      <c r="I96" s="35">
+      <c r="I97" s="20">
         <f t="shared" si="7"/>
         <v>-4.8161207980063573E-5</v>
       </c>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B97" s="6">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98" s="6">
         <v>670</v>
       </c>
-      <c r="C97" s="8">
+      <c r="C98" s="8">
         <v>3359.32</v>
       </c>
-      <c r="D97" s="8">
+      <c r="D98" s="8">
         <f t="shared" si="4"/>
         <v>335.93200000000002</v>
       </c>
-      <c r="E97" s="9">
+      <c r="E98" s="9">
         <v>1679.66</v>
       </c>
-      <c r="G97" s="35">
+      <c r="G98" s="20">
         <f t="shared" si="5"/>
         <v>669.99960120598212</v>
       </c>
-      <c r="H97" s="35">
+      <c r="H98" s="20">
         <f t="shared" si="6"/>
         <v>3.9879401788311952E-4</v>
       </c>
-      <c r="I97" s="35">
+      <c r="I98" s="20">
         <f t="shared" si="7"/>
         <v>5.9521495206435755E-5</v>
       </c>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B98" s="6">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99" s="6">
         <v>680</v>
       </c>
-      <c r="C98" s="8">
+      <c r="C99" s="8">
         <v>3390.61</v>
       </c>
-      <c r="D98" s="8">
+      <c r="D99" s="8">
         <f t="shared" si="4"/>
         <v>339.06100000000004</v>
       </c>
-      <c r="E98" s="9">
+      <c r="E99" s="9">
         <v>1695.3</v>
       </c>
-      <c r="G98" s="35">
+      <c r="G99" s="20">
         <f t="shared" si="5"/>
         <v>680.00064043044472</v>
       </c>
-      <c r="H98" s="35">
+      <c r="H99" s="20">
         <f t="shared" si="6"/>
         <v>-6.4043044471873145E-4</v>
       </c>
-      <c r="I98" s="35">
+      <c r="I99" s="20">
         <f t="shared" si="7"/>
         <v>-9.4180947752754636E-5</v>
       </c>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B99" s="6">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100" s="6">
         <v>690</v>
       </c>
-      <c r="C99" s="8">
+      <c r="C100" s="8">
         <v>3421.78</v>
       </c>
-      <c r="D99" s="8">
+      <c r="D100" s="8">
         <f t="shared" si="4"/>
         <v>342.178</v>
       </c>
-      <c r="E99" s="9">
+      <c r="E100" s="9">
         <v>1710.89</v>
       </c>
-      <c r="G99" s="35">
+      <c r="G100" s="20">
         <f t="shared" si="5"/>
         <v>690.00024105292971</v>
       </c>
-      <c r="H99" s="35">
+      <c r="H100" s="20">
         <f t="shared" si="6"/>
         <v>-2.4105292970943992E-4</v>
       </c>
-      <c r="I99" s="35">
+      <c r="I100" s="20">
         <f t="shared" si="7"/>
         <v>-3.493520720426666E-5</v>
       </c>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B100" s="6">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" s="6">
         <v>700</v>
       </c>
-      <c r="C100" s="8">
+      <c r="C101" s="8">
         <v>3452.84</v>
       </c>
-      <c r="D100" s="8">
+      <c r="D101" s="8">
         <f t="shared" si="4"/>
         <v>345.28399999999999</v>
       </c>
-      <c r="E100" s="9">
+      <c r="E101" s="9">
         <v>1726.42</v>
       </c>
-      <c r="G100" s="35">
+      <c r="G101" s="20">
         <f t="shared" si="5"/>
         <v>700.0016130077754</v>
       </c>
-      <c r="H100" s="35">
+      <c r="H101" s="20">
         <f t="shared" si="6"/>
         <v>-1.6130077754041849E-3</v>
       </c>
-      <c r="I100" s="35">
+      <c r="I101" s="20">
         <f t="shared" si="7"/>
         <v>-2.3042968220059786E-4</v>
       </c>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B101" s="6">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="6">
         <v>710</v>
       </c>
-      <c r="C101" s="8">
+      <c r="C102" s="8">
         <v>3483.78</v>
       </c>
-      <c r="D101" s="8">
+      <c r="D102" s="8">
         <f t="shared" si="4"/>
         <v>348.37800000000004</v>
       </c>
-      <c r="E101" s="9">
+      <c r="E102" s="9">
         <v>1741.89</v>
       </c>
-      <c r="G101" s="35">
+      <c r="G102" s="20">
         <f t="shared" si="5"/>
         <v>710.00153808835648</v>
       </c>
-      <c r="H101" s="35">
+      <c r="H102" s="20">
         <f t="shared" si="6"/>
         <v>-1.5380883564830583E-3</v>
       </c>
-      <c r="I101" s="35">
+      <c r="I102" s="20">
         <f t="shared" si="7"/>
         <v>-2.1663216288493779E-4</v>
       </c>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B102" s="6">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B103" s="6">
         <v>720</v>
       </c>
-      <c r="C102" s="8">
+      <c r="C103" s="8">
         <v>3514.6</v>
       </c>
-      <c r="D102" s="8">
+      <c r="D103" s="8">
         <f t="shared" si="4"/>
         <v>351.46</v>
       </c>
-      <c r="E102" s="9">
+      <c r="E103" s="9">
         <v>1757.3</v>
       </c>
-      <c r="G102" s="35">
+      <c r="G103" s="20">
         <f t="shared" si="5"/>
         <v>719.99999999999966</v>
       </c>
-      <c r="H102" s="35">
+      <c r="H103" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I102" s="35">
+      <c r="I103" s="20">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B103" s="6">
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B104" s="6">
         <v>730</v>
       </c>
-      <c r="C103" s="8">
+      <c r="C104" s="8">
         <v>3545.31</v>
       </c>
-      <c r="D103" s="8">
+      <c r="D104" s="8">
         <f t="shared" si="4"/>
         <v>354.53100000000001</v>
       </c>
-      <c r="E103" s="9">
+      <c r="E104" s="9">
         <v>1772.65</v>
       </c>
-      <c r="G103" s="35">
+      <c r="G104" s="20">
         <f t="shared" si="5"/>
         <v>730.00024468624167</v>
       </c>
-      <c r="H103" s="35">
+      <c r="H104" s="20">
         <f t="shared" si="6"/>
         <v>-2.4468624167184316E-4</v>
       </c>
-      <c r="I103" s="35">
+      <c r="I104" s="20">
         <f t="shared" si="7"/>
         <v>-3.351866324271824E-5</v>
       </c>
     </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B104" s="6">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" s="6">
         <v>740</v>
       </c>
-      <c r="C104" s="8">
+      <c r="C105" s="8">
         <v>3575.9</v>
       </c>
-      <c r="D104" s="8">
+      <c r="D105" s="8">
         <f t="shared" si="4"/>
         <v>357.59000000000003</v>
       </c>
-      <c r="E104" s="9">
+      <c r="E105" s="9">
         <v>1787.95</v>
       </c>
-      <c r="G104" s="35">
+      <c r="G105" s="20">
         <f t="shared" si="5"/>
         <v>739.99901755323447</v>
       </c>
-      <c r="H104" s="35">
+      <c r="H105" s="20">
         <f t="shared" si="6"/>
         <v>9.8244676553349564E-4</v>
       </c>
-      <c r="I104" s="35">
+      <c r="I105" s="20">
         <f t="shared" si="7"/>
         <v>1.3276307642344536E-4</v>
       </c>
     </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B105" s="6">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" s="6">
         <v>750</v>
       </c>
-      <c r="C105" s="8">
+      <c r="C106" s="8">
         <v>3606.38</v>
       </c>
-      <c r="D105" s="8">
+      <c r="D106" s="8">
         <f t="shared" si="4"/>
         <v>360.63800000000003</v>
       </c>
-      <c r="E105" s="9">
+      <c r="E106" s="9">
         <v>1803.19</v>
       </c>
-      <c r="G105" s="35">
+      <c r="G106" s="20">
         <f t="shared" si="5"/>
         <v>749.99958909291297</v>
       </c>
-      <c r="H105" s="35">
+      <c r="H106" s="20">
         <f t="shared" si="6"/>
         <v>4.1090708702995471E-4</v>
       </c>
-      <c r="I105" s="35">
+      <c r="I106" s="20">
         <f t="shared" si="7"/>
         <v>5.4787611603993954E-5</v>
       </c>
     </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B106" s="6">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" s="6">
         <v>760</v>
       </c>
-      <c r="C106" s="8">
+      <c r="C107" s="8">
         <v>3636.74</v>
       </c>
-      <c r="D106" s="8">
+      <c r="D107" s="8">
         <f t="shared" si="4"/>
         <v>363.67399999999998</v>
       </c>
-      <c r="E106" s="9">
+      <c r="E107" s="9">
         <v>1818.37</v>
       </c>
-      <c r="G106" s="35">
+      <c r="G107" s="20">
         <f t="shared" si="5"/>
         <v>759.99868008612577</v>
       </c>
-      <c r="H106" s="35">
+      <c r="H107" s="20">
         <f t="shared" si="6"/>
         <v>1.3199138742265859E-3</v>
       </c>
-      <c r="I106" s="35">
+      <c r="I107" s="20">
         <f t="shared" si="7"/>
         <v>1.7367287818770866E-4</v>
       </c>
     </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B107" s="6">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B108" s="6">
         <v>770</v>
       </c>
-      <c r="C107" s="8">
+      <c r="C108" s="8">
         <v>3666.99</v>
       </c>
-      <c r="D107" s="8">
+      <c r="D108" s="8">
         <f t="shared" si="4"/>
         <v>366.69899999999996</v>
       </c>
-      <c r="E107" s="9">
+      <c r="E108" s="9">
         <v>1833.5</v>
       </c>
-      <c r="G107" s="35">
+      <c r="G108" s="20">
         <f t="shared" si="5"/>
         <v>769.99958594878922</v>
       </c>
-      <c r="H107" s="35">
+      <c r="H108" s="20">
         <f t="shared" si="6"/>
         <v>4.1405121078241791E-4</v>
       </c>
-      <c r="I107" s="35">
+      <c r="I108" s="20">
         <f t="shared" si="7"/>
         <v>5.3772884517197129E-5</v>
       </c>
     </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B108" s="6">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109" s="6">
         <v>780</v>
       </c>
-      <c r="C108" s="8">
+      <c r="C109" s="8">
         <v>3697.12</v>
       </c>
-      <c r="D108" s="8">
+      <c r="D109" s="8">
         <f t="shared" si="4"/>
         <v>369.71199999999999</v>
       </c>
-      <c r="E108" s="9">
+      <c r="E109" s="9">
         <v>1848.56</v>
       </c>
-      <c r="G108" s="35">
+      <c r="G109" s="20">
         <f t="shared" si="5"/>
         <v>779.99900246078778</v>
       </c>
-      <c r="H108" s="35">
+      <c r="H109" s="20">
         <f t="shared" si="6"/>
         <v>9.9753921222145436E-4</v>
       </c>
-      <c r="I108" s="35">
+      <c r="I109" s="20">
         <f t="shared" si="7"/>
         <v>1.2788964259249414E-4</v>
       </c>
     </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B109" s="6">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110" s="6">
         <v>790</v>
       </c>
-      <c r="C109" s="8">
+      <c r="C110" s="8">
         <v>3727.14</v>
       </c>
-      <c r="D109" s="8">
+      <c r="D110" s="8">
         <f t="shared" si="4"/>
         <v>372.714</v>
       </c>
-      <c r="E109" s="9">
+      <c r="E110" s="9">
         <v>1863.57</v>
       </c>
-      <c r="G109" s="35">
+      <c r="G110" s="20">
         <f t="shared" si="5"/>
         <v>790.00025034632449</v>
       </c>
-      <c r="H109" s="35">
+      <c r="H110" s="20">
         <f t="shared" si="6"/>
         <v>-2.5034632449205674E-4</v>
       </c>
-      <c r="I109" s="35">
+      <c r="I110" s="20">
         <f t="shared" si="7"/>
         <v>-3.1689408163551488E-5</v>
       </c>
     </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B110" s="6">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B111" s="6">
         <v>800</v>
       </c>
-      <c r="C110" s="8">
+      <c r="C111" s="8">
         <v>3757.04</v>
       </c>
-      <c r="D110" s="8">
+      <c r="D111" s="8">
         <f t="shared" si="4"/>
         <v>375.70400000000001</v>
       </c>
-      <c r="E110" s="9">
+      <c r="E111" s="9">
         <v>1878.52</v>
       </c>
-      <c r="G110" s="35">
+      <c r="G111" s="20">
         <f t="shared" si="5"/>
         <v>800</v>
       </c>
-      <c r="H110" s="35">
+      <c r="H111" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I110" s="35">
+      <c r="I111" s="20">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B111" s="6">
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112" s="6">
         <v>810</v>
       </c>
-      <c r="C111" s="8">
+      <c r="C112" s="8">
         <v>3786.83</v>
       </c>
-      <c r="D111" s="8">
+      <c r="D112" s="8">
         <f t="shared" si="4"/>
         <v>378.68299999999999</v>
       </c>
-      <c r="E111" s="9">
+      <c r="E112" s="9">
         <v>1893.41</v>
       </c>
-      <c r="G111" s="35">
+      <c r="G112" s="20">
         <f t="shared" si="5"/>
         <v>810.00159784760683</v>
       </c>
-      <c r="H111" s="35">
+      <c r="H112" s="20">
         <f t="shared" si="6"/>
         <v>-1.5978476068312375E-3</v>
       </c>
-      <c r="I111" s="35">
+      <c r="I112" s="20">
         <f t="shared" si="7"/>
         <v>-1.9726513664583179E-4</v>
       </c>
     </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B112" s="6">
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="6">
         <v>820</v>
       </c>
-      <c r="C112" s="8">
+      <c r="C113" s="8">
         <v>3816.5</v>
       </c>
-      <c r="D112" s="8">
+      <c r="D113" s="8">
         <f t="shared" si="4"/>
         <v>381.65</v>
       </c>
-      <c r="E112" s="9">
+      <c r="E113" s="9">
         <v>1908.25</v>
       </c>
-      <c r="G112" s="35">
+      <c r="G113" s="20">
         <f t="shared" si="5"/>
         <v>820.00168850521607</v>
       </c>
-      <c r="H112" s="35">
+      <c r="H113" s="20">
         <f t="shared" si="6"/>
         <v>-1.6885052160660052E-3</v>
       </c>
-      <c r="I112" s="35">
+      <c r="I113" s="20">
         <f t="shared" si="7"/>
         <v>-2.0591527025195188E-4</v>
       </c>
     </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B113" s="6">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B114" s="6">
         <v>830</v>
       </c>
-      <c r="C113" s="8">
+      <c r="C114" s="8">
         <v>3846.05</v>
       </c>
-      <c r="D113" s="8">
+      <c r="D114" s="8">
         <f t="shared" si="4"/>
         <v>384.60500000000002</v>
       </c>
-      <c r="E113" s="9">
+      <c r="E114" s="9">
         <v>1923.02</v>
       </c>
-      <c r="G113" s="35">
+      <c r="G114" s="20">
         <f t="shared" si="5"/>
         <v>830.00025426746765</v>
       </c>
-      <c r="H113" s="35">
+      <c r="H114" s="20">
         <f t="shared" si="6"/>
         <v>-2.5426746765333519E-4</v>
       </c>
-      <c r="I113" s="35">
+      <c r="I114" s="20">
         <f t="shared" si="7"/>
         <v>-3.0634634657028339E-5</v>
       </c>
     </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B114" s="6">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B115" s="6">
         <v>840</v>
       </c>
-      <c r="C114" s="8">
+      <c r="C115" s="8">
         <v>3875.49</v>
       </c>
-      <c r="D114" s="8">
+      <c r="D115" s="8">
         <f t="shared" si="4"/>
         <v>387.54899999999998</v>
       </c>
-      <c r="E114" s="9">
+      <c r="E115" s="9">
         <v>1937.74</v>
       </c>
-      <c r="G114" s="35">
+      <c r="G115" s="20">
         <f t="shared" si="5"/>
         <v>840.00068071211558</v>
       </c>
-      <c r="H114" s="35">
+      <c r="H115" s="20">
         <f t="shared" si="6"/>
         <v>-6.8071211558162759E-4</v>
       </c>
-      <c r="I114" s="35">
+      <c r="I115" s="20">
         <f t="shared" si="7"/>
         <v>-8.1037156616860421E-5</v>
       </c>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B115" s="6">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B116" s="6">
         <v>850</v>
       </c>
-      <c r="C115" s="8">
+      <c r="C116" s="8">
         <v>3904.81</v>
       </c>
-      <c r="D115" s="8">
+      <c r="D116" s="8">
         <f t="shared" si="4"/>
         <v>390.48099999999999</v>
       </c>
-      <c r="E115" s="13"/>
-      <c r="G115" s="35">
+      <c r="E116" s="13"/>
+      <c r="G116" s="20">
         <f t="shared" si="5"/>
         <v>849.99957287594793</v>
       </c>
-      <c r="H115" s="35">
+      <c r="H116" s="20">
         <f t="shared" si="6"/>
         <v>4.2712405206657422E-4</v>
       </c>
-      <c r="I115" s="35">
+      <c r="I116" s="20">
         <f t="shared" si="7"/>
         <v>5.0249888478420494E-5</v>
       </c>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C116" s="5"/>
-    </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C117" s="5"/>
     </row>
@@ -9146,12 +9144,15 @@
     <row r="243" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C243" s="5"/>
     </row>
+    <row r="244" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C244" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:M2"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B2:M3"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>